<commit_message>
control stuff w mux
</commit_message>
<xml_diff>
--- a/ArquiProjecto/Phase2/ControlStateDiagram.xlsx
+++ b/ArquiProjecto/Phase2/ControlStateDiagram.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1563" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="197">
   <si>
     <t>BRANCH</t>
   </si>
@@ -1482,8 +1482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP213"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AG160" sqref="AG160:AJ160"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AG46" sqref="AG15:AG46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2503,9 +2503,7 @@
         <v>1</v>
       </c>
       <c r="AF15" s="13"/>
-      <c r="AG15" s="15" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG15" s="15"/>
       <c r="AH15" s="15" t="s">
         <v>29</v>
       </c>
@@ -2591,9 +2589,7 @@
         <v>1</v>
       </c>
       <c r="AF16" s="13"/>
-      <c r="AG16" s="14" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG16" s="14"/>
       <c r="AH16" s="14" t="s">
         <v>29</v>
       </c>
@@ -2681,9 +2677,7 @@
         <v>1</v>
       </c>
       <c r="AF17" s="13"/>
-      <c r="AG17" s="15" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG17" s="15"/>
       <c r="AH17" s="15" t="s">
         <v>29</v>
       </c>
@@ -2769,9 +2763,7 @@
         <v>1</v>
       </c>
       <c r="AF18" s="13"/>
-      <c r="AG18" s="14" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG18" s="14"/>
       <c r="AH18" s="14" t="s">
         <v>29</v>
       </c>
@@ -2859,9 +2851,7 @@
         <v>1</v>
       </c>
       <c r="AF19" s="13"/>
-      <c r="AG19" s="15" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG19" s="15"/>
       <c r="AH19" s="15" t="s">
         <v>29</v>
       </c>
@@ -2947,9 +2937,7 @@
         <v>1</v>
       </c>
       <c r="AF20" s="13"/>
-      <c r="AG20" s="14" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG20" s="14"/>
       <c r="AH20" s="14" t="s">
         <v>29</v>
       </c>
@@ -3037,9 +3025,7 @@
         <v>1</v>
       </c>
       <c r="AF21" s="13"/>
-      <c r="AG21" s="15" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG21" s="15"/>
       <c r="AH21" s="15" t="s">
         <v>29</v>
       </c>
@@ -3125,9 +3111,7 @@
         <v>1</v>
       </c>
       <c r="AF22" s="13"/>
-      <c r="AG22" s="14" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG22" s="14"/>
       <c r="AH22" s="14" t="s">
         <v>29</v>
       </c>
@@ -3215,9 +3199,7 @@
         <v>1</v>
       </c>
       <c r="AF23" s="13"/>
-      <c r="AG23" s="15" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG23" s="15"/>
       <c r="AH23" s="15" t="s">
         <v>29</v>
       </c>
@@ -3303,9 +3285,7 @@
         <v>1</v>
       </c>
       <c r="AF24" s="13"/>
-      <c r="AG24" s="14" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG24" s="14"/>
       <c r="AH24" s="14" t="s">
         <v>29</v>
       </c>
@@ -3393,9 +3373,7 @@
         <v>1</v>
       </c>
       <c r="AF25" s="13"/>
-      <c r="AG25" s="15" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG25" s="15"/>
       <c r="AH25" s="15" t="s">
         <v>29</v>
       </c>
@@ -3481,9 +3459,7 @@
         <v>1</v>
       </c>
       <c r="AF26" s="13"/>
-      <c r="AG26" s="14" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG26" s="14"/>
       <c r="AH26" s="14" t="s">
         <v>29</v>
       </c>
@@ -3571,9 +3547,7 @@
         <v>1</v>
       </c>
       <c r="AF27" s="13"/>
-      <c r="AG27" s="15" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG27" s="15"/>
       <c r="AH27" s="15" t="s">
         <v>29</v>
       </c>
@@ -3659,9 +3633,7 @@
         <v>1</v>
       </c>
       <c r="AF28" s="13"/>
-      <c r="AG28" s="14" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG28" s="14"/>
       <c r="AH28" s="14" t="s">
         <v>29</v>
       </c>
@@ -3749,9 +3721,7 @@
         <v>1</v>
       </c>
       <c r="AF29" s="13"/>
-      <c r="AG29" s="15" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG29" s="15"/>
       <c r="AH29" s="15" t="s">
         <v>29</v>
       </c>
@@ -3837,9 +3807,7 @@
         <v>1</v>
       </c>
       <c r="AF30" s="13"/>
-      <c r="AG30" s="14" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG30" s="14"/>
       <c r="AH30" s="14" t="s">
         <v>29</v>
       </c>
@@ -3927,9 +3895,7 @@
         <v>1</v>
       </c>
       <c r="AF31" s="13"/>
-      <c r="AG31" s="15" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG31" s="15"/>
       <c r="AH31" s="15" t="s">
         <v>29</v>
       </c>
@@ -4015,9 +3981,7 @@
         <v>1</v>
       </c>
       <c r="AF32" s="13"/>
-      <c r="AG32" s="14" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG32" s="14"/>
       <c r="AH32" s="14" t="s">
         <v>29</v>
       </c>
@@ -4105,9 +4069,7 @@
         <v>1</v>
       </c>
       <c r="AF33" s="13"/>
-      <c r="AG33" s="15" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG33" s="15"/>
       <c r="AH33" s="15" t="s">
         <v>29</v>
       </c>
@@ -4193,9 +4155,7 @@
         <v>1</v>
       </c>
       <c r="AF34" s="13"/>
-      <c r="AG34" s="14" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG34" s="14"/>
       <c r="AH34" s="14" t="s">
         <v>29</v>
       </c>
@@ -4283,9 +4243,7 @@
         <v>1</v>
       </c>
       <c r="AF35" s="13"/>
-      <c r="AG35" s="15" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG35" s="15"/>
       <c r="AH35" s="15" t="s">
         <v>29</v>
       </c>
@@ -4371,9 +4329,7 @@
         <v>1</v>
       </c>
       <c r="AF36" s="13"/>
-      <c r="AG36" s="14" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG36" s="14"/>
       <c r="AH36" s="14" t="s">
         <v>29</v>
       </c>
@@ -4461,9 +4417,7 @@
         <v>1</v>
       </c>
       <c r="AF37" s="13"/>
-      <c r="AG37" s="15" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG37" s="15"/>
       <c r="AH37" s="15" t="s">
         <v>29</v>
       </c>
@@ -4549,9 +4503,7 @@
         <v>1</v>
       </c>
       <c r="AF38" s="13"/>
-      <c r="AG38" s="14" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG38" s="14"/>
       <c r="AH38" s="14" t="s">
         <v>29</v>
       </c>
@@ -4639,9 +4591,7 @@
         <v>1</v>
       </c>
       <c r="AF39" s="13"/>
-      <c r="AG39" s="15" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG39" s="15"/>
       <c r="AH39" s="15" t="s">
         <v>29</v>
       </c>
@@ -4727,9 +4677,7 @@
         <v>1</v>
       </c>
       <c r="AF40" s="13"/>
-      <c r="AG40" s="14" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG40" s="14"/>
       <c r="AH40" s="14" t="s">
         <v>29</v>
       </c>
@@ -4817,9 +4765,7 @@
         <v>1</v>
       </c>
       <c r="AF41" s="13"/>
-      <c r="AG41" s="15" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG41" s="15"/>
       <c r="AH41" s="15" t="s">
         <v>29</v>
       </c>
@@ -4905,9 +4851,7 @@
         <v>1</v>
       </c>
       <c r="AF42" s="13"/>
-      <c r="AG42" s="14" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG42" s="14"/>
       <c r="AH42" s="14" t="s">
         <v>29</v>
       </c>
@@ -4995,9 +4939,7 @@
         <v>1</v>
       </c>
       <c r="AF43" s="13"/>
-      <c r="AG43" s="15" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG43" s="15"/>
       <c r="AH43" s="15" t="s">
         <v>29</v>
       </c>
@@ -5083,9 +5025,7 @@
         <v>1</v>
       </c>
       <c r="AF44" s="13"/>
-      <c r="AG44" s="14" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG44" s="14"/>
       <c r="AH44" s="14" t="s">
         <v>29</v>
       </c>
@@ -5173,9 +5113,7 @@
         <v>1</v>
       </c>
       <c r="AF45" s="13"/>
-      <c r="AG45" s="15" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG45" s="15"/>
       <c r="AH45" s="15" t="s">
         <v>29</v>
       </c>
@@ -5261,9 +5199,7 @@
         <v>1</v>
       </c>
       <c r="AF46" s="13"/>
-      <c r="AG46" s="14" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG46" s="14"/>
       <c r="AH46" s="14" t="s">
         <v>29</v>
       </c>
@@ -7130,9 +7066,7 @@
         <v>0</v>
       </c>
       <c r="AF79" s="13"/>
-      <c r="AG79" s="9" t="s">
-        <v>77</v>
-      </c>
+      <c r="AG79" s="9"/>
       <c r="AH79" s="9" t="s">
         <v>77</v>
       </c>
@@ -11028,9 +10962,7 @@
         <v>1</v>
       </c>
       <c r="AF150" s="13"/>
-      <c r="AG150" s="13" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG150" s="13"/>
       <c r="AH150" s="13" t="s">
         <v>29</v>
       </c>
@@ -11305,9 +11237,7 @@
         <v>0</v>
       </c>
       <c r="AF154" s="13"/>
-      <c r="AG154" s="13" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG154" s="13"/>
       <c r="AH154" s="13" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
cu and control state diagram update
</commit_message>
<xml_diff>
--- a/ArquiProjecto/Phase2/ControlStateDiagram.xlsx
+++ b/ArquiProjecto/Phase2/ControlStateDiagram.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hecto\Documents\armverilogimplementation\ArquiProjecto\Phase2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Desktop\Arqui\gitrepository\armverilogimplementation\ArquiProjecto\Phase2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -994,7 +994,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1221,19 +1221,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1519,17 +1519,17 @@
   </sheetPr>
   <dimension ref="A1:AQ211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P149" sqref="P149"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="28" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="28" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="28" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="28" customWidth="1"/>
     <col min="6" max="6" width="1.85546875" style="19" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
     <col min="8" max="8" width="1.85546875" style="19" customWidth="1"/>
@@ -1555,12 +1555,12 @@
       <c r="A2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
@@ -1574,11 +1574,11 @@
       <c r="N2" s="43"/>
       <c r="O2" s="43"/>
       <c r="P2" s="13"/>
-      <c r="Q2" s="42" t="s">
+      <c r="Q2" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="R2" s="42"/>
-      <c r="S2" s="42"/>
+      <c r="R2" s="45"/>
+      <c r="S2" s="45"/>
       <c r="T2" s="13"/>
       <c r="U2" s="7" t="s">
         <v>67</v>
@@ -2257,23 +2257,23 @@
       <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="45"/>
-      <c r="L11" s="45"/>
-      <c r="M11" s="45"/>
-      <c r="N11" s="45"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="46"/>
       <c r="O11" s="13"/>
       <c r="P11" s="13"/>
-      <c r="Q11" s="45"/>
-      <c r="R11" s="45"/>
+      <c r="Q11" s="46"/>
+      <c r="R11" s="46"/>
       <c r="S11" s="13"/>
       <c r="T11" s="13"/>
       <c r="U11" s="8"/>
@@ -2283,26 +2283,26 @@
       <c r="Z11" s="13"/>
       <c r="AA11" s="13"/>
       <c r="AB11" s="13"/>
-      <c r="AC11" s="45"/>
-      <c r="AD11" s="45"/>
+      <c r="AC11" s="46"/>
+      <c r="AD11" s="46"/>
       <c r="AE11" s="23"/>
       <c r="AF11" s="13"/>
       <c r="AG11" s="13"/>
       <c r="AH11" s="13"/>
-      <c r="AI11" s="45"/>
-      <c r="AJ11" s="45"/>
-      <c r="AK11" s="45"/>
+      <c r="AI11" s="46"/>
+      <c r="AJ11" s="46"/>
+      <c r="AK11" s="46"/>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
@@ -2316,11 +2316,11 @@
       <c r="N12" s="43"/>
       <c r="O12" s="43"/>
       <c r="P12" s="13"/>
-      <c r="Q12" s="42" t="s">
+      <c r="Q12" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="R12" s="42"/>
-      <c r="S12" s="42"/>
+      <c r="R12" s="45"/>
+      <c r="S12" s="45"/>
       <c r="T12" s="13"/>
       <c r="U12" s="7" t="s">
         <v>67</v>
@@ -5557,12 +5557,12 @@
       <c r="A49" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B49" s="42" t="s">
+      <c r="B49" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="C49" s="42"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="42"/>
+      <c r="C49" s="45"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="45"/>
       <c r="F49" s="20"/>
       <c r="G49" s="20"/>
       <c r="H49" s="20"/>
@@ -5576,11 +5576,11 @@
       <c r="N49" s="43"/>
       <c r="O49" s="43"/>
       <c r="P49" s="13"/>
-      <c r="Q49" s="42" t="s">
+      <c r="Q49" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="R49" s="42"/>
-      <c r="S49" s="42"/>
+      <c r="R49" s="45"/>
+      <c r="S49" s="45"/>
       <c r="T49" s="13"/>
       <c r="U49" s="7" t="s">
         <v>67</v>
@@ -8134,12 +8134,12 @@
       <c r="A81" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B81" s="42" t="s">
+      <c r="B81" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="C81" s="42"/>
-      <c r="D81" s="42"/>
-      <c r="E81" s="42"/>
+      <c r="C81" s="45"/>
+      <c r="D81" s="45"/>
+      <c r="E81" s="45"/>
       <c r="F81" s="20"/>
       <c r="G81" s="20"/>
       <c r="H81" s="20"/>
@@ -8153,11 +8153,11 @@
       <c r="N81" s="43"/>
       <c r="O81" s="43"/>
       <c r="P81" s="13"/>
-      <c r="Q81" s="42" t="s">
+      <c r="Q81" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="R81" s="42"/>
-      <c r="S81" s="42"/>
+      <c r="R81" s="45"/>
+      <c r="S81" s="45"/>
       <c r="T81" s="13"/>
       <c r="U81" s="7" t="s">
         <v>67</v>
@@ -10711,12 +10711,12 @@
       <c r="A113" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B113" s="42" t="s">
+      <c r="B113" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="C113" s="42"/>
-      <c r="D113" s="42"/>
-      <c r="E113" s="42"/>
+      <c r="C113" s="45"/>
+      <c r="D113" s="45"/>
+      <c r="E113" s="45"/>
       <c r="F113" s="20"/>
       <c r="G113" s="20"/>
       <c r="H113" s="20"/>
@@ -10730,11 +10730,11 @@
       <c r="N113" s="43"/>
       <c r="O113" s="43"/>
       <c r="P113" s="13"/>
-      <c r="Q113" s="42" t="s">
+      <c r="Q113" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="R113" s="42"/>
-      <c r="S113" s="42"/>
+      <c r="R113" s="45"/>
+      <c r="S113" s="45"/>
       <c r="T113" s="13"/>
       <c r="U113" s="7" t="s">
         <v>67</v>
@@ -12142,12 +12142,12 @@
       <c r="A131" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B131" s="42" t="s">
+      <c r="B131" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="C131" s="42"/>
-      <c r="D131" s="42"/>
-      <c r="E131" s="42"/>
+      <c r="C131" s="45"/>
+      <c r="D131" s="45"/>
+      <c r="E131" s="45"/>
       <c r="F131" s="20"/>
       <c r="G131" s="20"/>
       <c r="H131" s="20"/>
@@ -12161,11 +12161,11 @@
       <c r="N131" s="43"/>
       <c r="O131" s="43"/>
       <c r="P131" s="13"/>
-      <c r="Q131" s="42" t="s">
+      <c r="Q131" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="R131" s="42"/>
-      <c r="S131" s="42"/>
+      <c r="R131" s="45"/>
+      <c r="S131" s="45"/>
       <c r="T131" s="13"/>
       <c r="U131" s="7" t="s">
         <v>67</v>
@@ -13532,12 +13532,12 @@
       <c r="A148" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B148" s="42" t="s">
+      <c r="B148" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="C148" s="42"/>
-      <c r="D148" s="42"/>
-      <c r="E148" s="42"/>
+      <c r="C148" s="45"/>
+      <c r="D148" s="45"/>
+      <c r="E148" s="45"/>
       <c r="F148" s="20"/>
       <c r="G148" s="20"/>
       <c r="H148" s="20"/>
@@ -13551,11 +13551,11 @@
       <c r="N148" s="43"/>
       <c r="O148" s="43"/>
       <c r="P148" s="13"/>
-      <c r="Q148" s="42" t="s">
+      <c r="Q148" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="R148" s="42"/>
-      <c r="S148" s="42"/>
+      <c r="R148" s="45"/>
+      <c r="S148" s="45"/>
       <c r="T148" s="13"/>
       <c r="U148" s="7" t="s">
         <v>67</v>
@@ -13817,12 +13817,12 @@
       <c r="A152" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B152" s="42" t="s">
+      <c r="B152" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="C152" s="42"/>
-      <c r="D152" s="42"/>
-      <c r="E152" s="42"/>
+      <c r="C152" s="45"/>
+      <c r="D152" s="45"/>
+      <c r="E152" s="45"/>
       <c r="F152" s="20"/>
       <c r="G152" s="20"/>
       <c r="H152" s="20"/>
@@ -13836,11 +13836,11 @@
       <c r="N152" s="43"/>
       <c r="O152" s="43"/>
       <c r="P152" s="13"/>
-      <c r="Q152" s="42" t="s">
+      <c r="Q152" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="R152" s="42"/>
-      <c r="S152" s="42"/>
+      <c r="R152" s="45"/>
+      <c r="S152" s="45"/>
       <c r="T152" s="13"/>
       <c r="U152" s="7" t="s">
         <v>67</v>
@@ -14101,12 +14101,12 @@
       <c r="A156" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B156" s="42" t="s">
+      <c r="B156" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="C156" s="42"/>
-      <c r="D156" s="42"/>
-      <c r="E156" s="42"/>
+      <c r="C156" s="45"/>
+      <c r="D156" s="45"/>
+      <c r="E156" s="45"/>
       <c r="F156" s="20"/>
       <c r="G156" s="20"/>
       <c r="H156" s="20"/>
@@ -14120,11 +14120,11 @@
       <c r="N156" s="43"/>
       <c r="O156" s="43"/>
       <c r="P156" s="13"/>
-      <c r="Q156" s="42" t="s">
+      <c r="Q156" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="R156" s="42"/>
-      <c r="S156" s="42"/>
+      <c r="R156" s="45"/>
+      <c r="S156" s="45"/>
       <c r="T156" s="13"/>
       <c r="U156" s="7" t="s">
         <v>67</v>
@@ -14338,12 +14338,12 @@
       <c r="A160" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B160" s="42" t="s">
+      <c r="B160" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="C160" s="42"/>
-      <c r="D160" s="42"/>
-      <c r="E160" s="42"/>
+      <c r="C160" s="45"/>
+      <c r="D160" s="45"/>
+      <c r="E160" s="45"/>
       <c r="F160" s="20"/>
       <c r="G160" s="20"/>
       <c r="H160" s="20"/>
@@ -14357,11 +14357,11 @@
       <c r="N160" s="43"/>
       <c r="O160" s="43"/>
       <c r="P160" s="13"/>
-      <c r="Q160" s="42" t="s">
+      <c r="Q160" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="R160" s="42"/>
-      <c r="S160" s="42"/>
+      <c r="R160" s="45"/>
+      <c r="S160" s="45"/>
       <c r="T160" s="13"/>
       <c r="U160" s="7" t="s">
         <v>67</v>
@@ -14582,7 +14582,7 @@
       <c r="AL166" s="8"/>
     </row>
     <row r="167" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A167" s="46"/>
+      <c r="A167" s="42"/>
       <c r="AL167" s="8"/>
     </row>
     <row r="168" spans="1:38" x14ac:dyDescent="0.25">
@@ -14719,6 +14719,46 @@
     </row>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="B160:E160"/>
+    <mergeCell ref="AC160:AD160"/>
+    <mergeCell ref="AH160:AK160"/>
+    <mergeCell ref="I160:O160"/>
+    <mergeCell ref="Q160:S160"/>
+    <mergeCell ref="B156:E156"/>
+    <mergeCell ref="AC156:AD156"/>
+    <mergeCell ref="AH156:AK156"/>
+    <mergeCell ref="I156:O156"/>
+    <mergeCell ref="Q156:S156"/>
+    <mergeCell ref="AH12:AK12"/>
+    <mergeCell ref="AH49:AK49"/>
+    <mergeCell ref="AI11:AK11"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="I49:O49"/>
+    <mergeCell ref="I12:O12"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="Q49:S49"/>
+    <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="AC11:AD11"/>
+    <mergeCell ref="B148:E148"/>
+    <mergeCell ref="B152:E152"/>
+    <mergeCell ref="AC148:AD148"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="I11:N11"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="AC12:AD12"/>
+    <mergeCell ref="B131:E131"/>
+    <mergeCell ref="AH131:AK131"/>
+    <mergeCell ref="I81:O81"/>
+    <mergeCell ref="I113:O113"/>
+    <mergeCell ref="I131:O131"/>
+    <mergeCell ref="Q81:S81"/>
+    <mergeCell ref="Q113:S113"/>
+    <mergeCell ref="Q131:S131"/>
     <mergeCell ref="AC152:AD152"/>
     <mergeCell ref="D47:AI47"/>
     <mergeCell ref="AC131:AD131"/>
@@ -14735,46 +14775,6 @@
     <mergeCell ref="AH81:AK81"/>
     <mergeCell ref="B113:E113"/>
     <mergeCell ref="AH113:AK113"/>
-    <mergeCell ref="B131:E131"/>
-    <mergeCell ref="AH131:AK131"/>
-    <mergeCell ref="I81:O81"/>
-    <mergeCell ref="I113:O113"/>
-    <mergeCell ref="I131:O131"/>
-    <mergeCell ref="Q81:S81"/>
-    <mergeCell ref="Q113:S113"/>
-    <mergeCell ref="Q131:S131"/>
-    <mergeCell ref="B148:E148"/>
-    <mergeCell ref="B152:E152"/>
-    <mergeCell ref="AC148:AD148"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="I11:N11"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="AC11:AD11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="AC12:AD12"/>
-    <mergeCell ref="AH12:AK12"/>
-    <mergeCell ref="AH49:AK49"/>
-    <mergeCell ref="AI11:AK11"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="I49:O49"/>
-    <mergeCell ref="I12:O12"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="Q49:S49"/>
-    <mergeCell ref="B156:E156"/>
-    <mergeCell ref="AC156:AD156"/>
-    <mergeCell ref="AH156:AK156"/>
-    <mergeCell ref="I156:O156"/>
-    <mergeCell ref="Q156:S156"/>
-    <mergeCell ref="B160:E160"/>
-    <mergeCell ref="AC160:AD160"/>
-    <mergeCell ref="AH160:AK160"/>
-    <mergeCell ref="I160:O160"/>
-    <mergeCell ref="Q160:S160"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="44" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Stop spying on me Big Brother!
</commit_message>
<xml_diff>
--- a/ArquiProjecto/Phase2/ControlStateDiagram.xlsx
+++ b/ArquiProjecto/Phase2/ControlStateDiagram.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hecto\Documents\Github Files\ARMVerilogImplementation\ArquiProjecto\Phase2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hecto\Documents\armverilogimplementation\ArquiProjecto\Phase2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12798" windowHeight="4038"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12795" windowHeight="4035"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2226" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2217" uniqueCount="194">
   <si>
     <t>BRANCH</t>
   </si>
@@ -883,12 +883,6 @@
     <t>Rn=Rn-Rm - 69</t>
   </si>
   <si>
-    <t>mfc wait - 70</t>
-  </si>
-  <si>
-    <t>save in ram - 71</t>
-  </si>
-  <si>
     <t>EA=Rn+offset_8 - 72</t>
   </si>
   <si>
@@ -931,12 +925,6 @@
     <t>Rn=Rn-offset_8 - 89</t>
   </si>
   <si>
-    <t>mfc wait - 90</t>
-  </si>
-  <si>
-    <t>save in ram - 91</t>
-  </si>
-  <si>
     <t>Rn=Rn+offset_8 - 87</t>
   </si>
   <si>
@@ -968,12 +956,30 @@
   </si>
   <si>
     <t>00</t>
+  </si>
+  <si>
+    <t>EA=Rn+offset_12 - 54</t>
+  </si>
+  <si>
+    <t>EA=Rn-offset_12 - 55</t>
+  </si>
+  <si>
+    <t>mfc wait - 71</t>
+  </si>
+  <si>
+    <t>save in ram - 70</t>
+  </si>
+  <si>
+    <t>save in ram - 90</t>
+  </si>
+  <si>
+    <t>mfc wait - 91</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1093,7 +1099,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -1200,6 +1206,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1211,6 +1220,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1497,68 +1509,68 @@
   </sheetPr>
   <dimension ref="A1:AQ211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L122" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AL144" sqref="AL144"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.26171875" customWidth="1"/>
-    <col min="2" max="2" width="9.15625" customWidth="1"/>
-    <col min="3" max="3" width="9.83984375" style="8" customWidth="1"/>
+    <col min="1" max="1" width="48.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="8" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="10.41796875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" style="19" customWidth="1"/>
-    <col min="7" max="7" width="5.68359375" customWidth="1"/>
-    <col min="8" max="8" width="1.83984375" style="19" customWidth="1"/>
-    <col min="9" max="9" width="11.68359375" customWidth="1"/>
-    <col min="16" max="16" width="1.83984375" style="8" customWidth="1"/>
-    <col min="20" max="20" width="1.83984375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" style="19" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" customWidth="1"/>
+    <col min="8" max="8" width="1.85546875" style="19" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="16" max="16" width="1.85546875" style="8" customWidth="1"/>
+    <col min="20" max="20" width="1.85546875" style="8" customWidth="1"/>
     <col min="21" max="21" width="10" customWidth="1"/>
-    <col min="22" max="22" width="1.68359375" style="8" customWidth="1"/>
-    <col min="24" max="24" width="1.83984375" style="8" customWidth="1"/>
-    <col min="26" max="26" width="1.83984375" style="8" customWidth="1"/>
-    <col min="28" max="28" width="1.83984375" style="8" customWidth="1"/>
-    <col min="31" max="31" width="1.83984375" style="8" customWidth="1"/>
-    <col min="33" max="33" width="1.83984375" style="8" customWidth="1"/>
-    <col min="34" max="35" width="10.41796875" customWidth="1"/>
+    <col min="22" max="22" width="1.7109375" style="8" customWidth="1"/>
+    <col min="24" max="24" width="1.85546875" style="8" customWidth="1"/>
+    <col min="26" max="26" width="1.85546875" style="8" customWidth="1"/>
+    <col min="28" max="28" width="1.85546875" style="8" customWidth="1"/>
+    <col min="31" max="31" width="1.85546875" style="8" customWidth="1"/>
+    <col min="33" max="33" width="1.85546875" style="8" customWidth="1"/>
+    <col min="34" max="35" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B1" s="8"/>
       <c r="D1" s="8"/>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
-      <c r="I2" s="43" t="s">
+      <c r="I2" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
       <c r="P2" s="13"/>
-      <c r="Q2" s="42" t="s">
+      <c r="Q2" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="R2" s="42"/>
-      <c r="S2" s="42"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
       <c r="T2" s="13"/>
       <c r="U2" s="7" t="s">
         <v>67</v>
@@ -1575,23 +1587,23 @@
         <v>70</v>
       </c>
       <c r="AB2" s="13"/>
-      <c r="AC2" s="43" t="s">
+      <c r="AC2" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="AD2" s="43"/>
+      <c r="AD2" s="44"/>
       <c r="AE2" s="23"/>
       <c r="AF2" s="18" t="s">
         <v>72</v>
       </c>
       <c r="AG2" s="13"/>
-      <c r="AH2" s="43" t="s">
+      <c r="AH2" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AI2" s="43"/>
-      <c r="AJ2" s="43"/>
-      <c r="AK2" s="43"/>
-    </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.55000000000000004">
+      <c r="AI2" s="44"/>
+      <c r="AJ2" s="44"/>
+      <c r="AK2" s="44"/>
+    </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -1631,7 +1643,7 @@
         <v>11</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P3" s="13"/>
       <c r="Q3" s="11" t="s">
@@ -1684,7 +1696,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>36</v>
       </c>
@@ -1777,7 +1789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>32</v>
       </c>
@@ -1870,9 +1882,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>28</v>
@@ -1901,7 +1913,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="35" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="M6" s="35" t="s">
         <v>28</v>
@@ -1964,7 +1976,7 @@
       </c>
       <c r="AQ6" s="26"/>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>33</v>
       </c>
@@ -2045,7 +2057,7 @@
       </c>
       <c r="AG7" s="36"/>
       <c r="AH7" s="37" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="AI7" s="35" t="s">
         <v>74</v>
@@ -2057,7 +2069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>34</v>
       </c>
@@ -2151,7 +2163,7 @@
       </c>
       <c r="AL8" s="8"/>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="13"/>
       <c r="C9" s="40"/>
@@ -2191,7 +2203,7 @@
       <c r="AK9" s="13"/>
       <c r="AL9" s="8"/>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
@@ -2233,27 +2245,27 @@
       <c r="AK10" s="13"/>
       <c r="AL10" s="8"/>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="44"/>
-      <c r="N11" s="44"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="45"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="45"/>
+      <c r="N11" s="45"/>
       <c r="O11" s="13"/>
       <c r="P11" s="13"/>
-      <c r="Q11" s="44"/>
-      <c r="R11" s="44"/>
+      <c r="Q11" s="45"/>
+      <c r="R11" s="45"/>
       <c r="S11" s="13"/>
       <c r="T11" s="13"/>
       <c r="U11" s="8"/>
@@ -2263,44 +2275,44 @@
       <c r="Z11" s="13"/>
       <c r="AA11" s="13"/>
       <c r="AB11" s="13"/>
-      <c r="AC11" s="44"/>
-      <c r="AD11" s="44"/>
+      <c r="AC11" s="45"/>
+      <c r="AD11" s="45"/>
       <c r="AE11" s="23"/>
       <c r="AF11" s="13"/>
       <c r="AG11" s="13"/>
       <c r="AH11" s="13"/>
-      <c r="AI11" s="44"/>
-      <c r="AJ11" s="44"/>
-      <c r="AK11" s="44"/>
-    </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.55000000000000004">
+      <c r="AI11" s="45"/>
+      <c r="AJ11" s="45"/>
+      <c r="AK11" s="45"/>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
-      <c r="I12" s="43" t="s">
+      <c r="I12" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="43"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="43"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="44"/>
+      <c r="M12" s="44"/>
+      <c r="N12" s="44"/>
+      <c r="O12" s="44"/>
       <c r="P12" s="13"/>
-      <c r="Q12" s="42" t="s">
+      <c r="Q12" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="R12" s="42"/>
-      <c r="S12" s="42"/>
+      <c r="R12" s="43"/>
+      <c r="S12" s="43"/>
       <c r="T12" s="13"/>
       <c r="U12" s="7" t="s">
         <v>67</v>
@@ -2317,23 +2329,23 @@
         <v>70</v>
       </c>
       <c r="AB12" s="13"/>
-      <c r="AC12" s="43" t="s">
+      <c r="AC12" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="AD12" s="43"/>
+      <c r="AD12" s="44"/>
       <c r="AE12" s="23"/>
       <c r="AF12" s="18" t="s">
         <v>72</v>
       </c>
       <c r="AG12" s="13"/>
-      <c r="AH12" s="43" t="s">
+      <c r="AH12" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AI12" s="43"/>
-      <c r="AJ12" s="43"/>
-      <c r="AK12" s="43"/>
-    </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.55000000000000004">
+      <c r="AI12" s="44"/>
+      <c r="AJ12" s="44"/>
+      <c r="AK12" s="44"/>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
@@ -2373,7 +2385,7 @@
         <v>11</v>
       </c>
       <c r="O13" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P13" s="13"/>
       <c r="Q13" s="11" t="s">
@@ -2431,7 +2443,7 @@
       <c r="AO13" s="8"/>
       <c r="AP13" s="8"/>
     </row>
-    <row r="14" spans="1:43" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:43" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="13"/>
       <c r="C14" s="40"/>
@@ -2470,7 +2482,7 @@
       <c r="AJ14" s="13"/>
       <c r="AK14" s="13"/>
     </row>
-    <row r="15" spans="1:43" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:43" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>87</v>
       </c>
@@ -2563,7 +2575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:43" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:43" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>88</v>
       </c>
@@ -2656,7 +2668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>89</v>
       </c>
@@ -2749,7 +2761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>90</v>
       </c>
@@ -2842,7 +2854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>91</v>
       </c>
@@ -2935,7 +2947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>103</v>
       </c>
@@ -3028,7 +3040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>92</v>
       </c>
@@ -3121,7 +3133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>104</v>
       </c>
@@ -3214,7 +3226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>93</v>
       </c>
@@ -3307,7 +3319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>105</v>
       </c>
@@ -3400,7 +3412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>94</v>
       </c>
@@ -3493,7 +3505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>106</v>
       </c>
@@ -3586,7 +3598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>95</v>
       </c>
@@ -3679,7 +3691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>107</v>
       </c>
@@ -3772,7 +3784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>96</v>
       </c>
@@ -3865,7 +3877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>108</v>
       </c>
@@ -3958,7 +3970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>97</v>
       </c>
@@ -4051,7 +4063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>109</v>
       </c>
@@ -4144,7 +4156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>98</v>
       </c>
@@ -4237,7 +4249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>110</v>
       </c>
@@ -4330,7 +4342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>99</v>
       </c>
@@ -4423,7 +4435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>111</v>
       </c>
@@ -4516,7 +4528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>100</v>
       </c>
@@ -4609,7 +4621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
         <v>112</v>
       </c>
@@ -4702,7 +4714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>101</v>
       </c>
@@ -4795,7 +4807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>113</v>
       </c>
@@ -4888,7 +4900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>102</v>
       </c>
@@ -4981,7 +4993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>114</v>
       </c>
@@ -5074,7 +5086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>116</v>
       </c>
@@ -5167,7 +5179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>117</v>
       </c>
@@ -5260,7 +5272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>115</v>
       </c>
@@ -5353,7 +5365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
         <v>118</v>
       </c>
@@ -5446,44 +5458,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16"/>
       <c r="B47" s="13"/>
       <c r="C47" s="40"/>
-      <c r="D47" s="45" t="s">
+      <c r="D47" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="E47" s="45"/>
-      <c r="F47" s="45"/>
-      <c r="G47" s="45"/>
-      <c r="H47" s="45"/>
-      <c r="I47" s="45"/>
-      <c r="J47" s="45"/>
-      <c r="K47" s="45"/>
-      <c r="L47" s="45"/>
-      <c r="M47" s="45"/>
-      <c r="N47" s="45"/>
-      <c r="O47" s="45"/>
-      <c r="P47" s="45"/>
-      <c r="Q47" s="45"/>
-      <c r="R47" s="45"/>
-      <c r="S47" s="45"/>
-      <c r="T47" s="45"/>
-      <c r="U47" s="45"/>
-      <c r="V47" s="45"/>
-      <c r="W47" s="45"/>
-      <c r="X47" s="45"/>
-      <c r="Y47" s="45"/>
-      <c r="Z47" s="45"/>
-      <c r="AA47" s="45"/>
-      <c r="AB47" s="45"/>
-      <c r="AC47" s="45"/>
-      <c r="AD47" s="45"/>
-      <c r="AE47" s="45"/>
-      <c r="AF47" s="45"/>
-      <c r="AG47" s="45"/>
-      <c r="AH47" s="45"/>
-      <c r="AI47" s="45"/>
+      <c r="E47" s="46"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="46"/>
+      <c r="I47" s="46"/>
+      <c r="J47" s="46"/>
+      <c r="K47" s="46"/>
+      <c r="L47" s="46"/>
+      <c r="M47" s="46"/>
+      <c r="N47" s="46"/>
+      <c r="O47" s="46"/>
+      <c r="P47" s="46"/>
+      <c r="Q47" s="46"/>
+      <c r="R47" s="46"/>
+      <c r="S47" s="46"/>
+      <c r="T47" s="46"/>
+      <c r="U47" s="46"/>
+      <c r="V47" s="46"/>
+      <c r="W47" s="46"/>
+      <c r="X47" s="46"/>
+      <c r="Y47" s="46"/>
+      <c r="Z47" s="46"/>
+      <c r="AA47" s="46"/>
+      <c r="AB47" s="46"/>
+      <c r="AC47" s="46"/>
+      <c r="AD47" s="46"/>
+      <c r="AE47" s="46"/>
+      <c r="AF47" s="46"/>
+      <c r="AG47" s="46"/>
+      <c r="AH47" s="46"/>
+      <c r="AI47" s="46"/>
       <c r="AJ47" s="13"/>
       <c r="AK47" s="13"/>
       <c r="AL47"/>
@@ -5492,7 +5504,7 @@
       <c r="AO47"/>
       <c r="AP47"/>
     </row>
-    <row r="48" spans="1:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>119</v>
       </c>
@@ -5533,34 +5545,34 @@
       <c r="AJ48" s="9"/>
       <c r="AK48" s="9"/>
     </row>
-    <row r="49" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B49" s="42" t="s">
+      <c r="B49" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="C49" s="42"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="42"/>
+      <c r="C49" s="43"/>
+      <c r="D49" s="43"/>
+      <c r="E49" s="43"/>
       <c r="F49" s="20"/>
       <c r="G49" s="20"/>
       <c r="H49" s="20"/>
-      <c r="I49" s="43" t="s">
+      <c r="I49" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="J49" s="43"/>
-      <c r="K49" s="43"/>
-      <c r="L49" s="43"/>
-      <c r="M49" s="43"/>
-      <c r="N49" s="43"/>
-      <c r="O49" s="43"/>
+      <c r="J49" s="44"/>
+      <c r="K49" s="44"/>
+      <c r="L49" s="44"/>
+      <c r="M49" s="44"/>
+      <c r="N49" s="44"/>
+      <c r="O49" s="44"/>
       <c r="P49" s="13"/>
-      <c r="Q49" s="42" t="s">
+      <c r="Q49" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="R49" s="42"/>
-      <c r="S49" s="42"/>
+      <c r="R49" s="43"/>
+      <c r="S49" s="43"/>
       <c r="T49" s="13"/>
       <c r="U49" s="7" t="s">
         <v>67</v>
@@ -5577,23 +5589,23 @@
         <v>70</v>
       </c>
       <c r="AB49" s="13"/>
-      <c r="AC49" s="43" t="s">
+      <c r="AC49" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="AD49" s="43"/>
+      <c r="AD49" s="44"/>
       <c r="AE49" s="23"/>
       <c r="AF49" s="18" t="s">
         <v>72</v>
       </c>
       <c r="AG49" s="13"/>
-      <c r="AH49" s="43" t="s">
+      <c r="AH49" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AI49" s="43"/>
-      <c r="AJ49" s="43"/>
-      <c r="AK49" s="43"/>
-    </row>
-    <row r="50" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+      <c r="AI49" s="44"/>
+      <c r="AJ49" s="44"/>
+      <c r="AK49" s="44"/>
+    </row>
+    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>25</v>
       </c>
@@ -5633,7 +5645,7 @@
         <v>11</v>
       </c>
       <c r="O50" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P50" s="13"/>
       <c r="Q50" s="11" t="s">
@@ -5686,7 +5698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
         <v>121</v>
       </c>
@@ -5700,7 +5712,7 @@
         <v>29</v>
       </c>
       <c r="E51" s="34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F51" s="20"/>
       <c r="G51" s="9">
@@ -5779,7 +5791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
         <v>125</v>
       </c>
@@ -5793,7 +5805,7 @@
         <v>29</v>
       </c>
       <c r="E52" s="34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F52" s="20"/>
       <c r="G52" s="9">
@@ -5872,7 +5884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>6</v>
       </c>
@@ -5913,7 +5925,7 @@
       <c r="AJ53" s="9"/>
       <c r="AK53" s="9"/>
     </row>
-    <row r="54" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>25</v>
       </c>
@@ -5953,7 +5965,7 @@
         <v>11</v>
       </c>
       <c r="O54" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P54" s="13"/>
       <c r="Q54" s="11" t="s">
@@ -6006,7 +6018,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
         <v>126</v>
       </c>
@@ -6020,7 +6032,7 @@
         <v>29</v>
       </c>
       <c r="E55" s="34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F55" s="20"/>
       <c r="G55" s="9">
@@ -6099,7 +6111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
         <v>127</v>
       </c>
@@ -6113,7 +6125,7 @@
         <v>29</v>
       </c>
       <c r="E56" s="34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F56" s="20"/>
       <c r="G56" s="9">
@@ -6192,7 +6204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>4</v>
       </c>
@@ -6233,7 +6245,7 @@
       <c r="AJ57" s="9"/>
       <c r="AK57" s="9"/>
     </row>
-    <row r="58" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>25</v>
       </c>
@@ -6273,7 +6285,7 @@
         <v>11</v>
       </c>
       <c r="O58" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P58" s="13"/>
       <c r="Q58" s="11" t="s">
@@ -6326,7 +6338,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
         <v>141</v>
       </c>
@@ -6340,7 +6352,7 @@
         <v>29</v>
       </c>
       <c r="E59" s="34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F59" s="20"/>
       <c r="G59" s="9">
@@ -6419,7 +6431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
         <v>142</v>
       </c>
@@ -6433,7 +6445,7 @@
         <v>29</v>
       </c>
       <c r="E60" s="34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F60" s="20"/>
       <c r="G60" s="9">
@@ -6512,7 +6524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
@@ -6553,7 +6565,7 @@
       <c r="AJ61" s="9"/>
       <c r="AK61" s="9"/>
     </row>
-    <row r="62" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>25</v>
       </c>
@@ -6593,7 +6605,7 @@
         <v>11</v>
       </c>
       <c r="O62" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P62" s="13"/>
       <c r="Q62" s="11" t="s">
@@ -6646,7 +6658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
         <v>143</v>
       </c>
@@ -6660,7 +6672,7 @@
         <v>29</v>
       </c>
       <c r="E63" s="34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F63" s="20"/>
       <c r="G63" s="9">
@@ -6739,7 +6751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A64" s="16" t="s">
         <v>144</v>
       </c>
@@ -6753,7 +6765,7 @@
         <v>29</v>
       </c>
       <c r="E64" s="34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F64" s="20"/>
       <c r="G64" s="9">
@@ -6832,7 +6844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>5</v>
       </c>
@@ -6873,7 +6885,7 @@
       <c r="AJ65" s="9"/>
       <c r="AK65" s="9"/>
     </row>
-    <row r="66" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>25</v>
       </c>
@@ -6913,7 +6925,7 @@
         <v>11</v>
       </c>
       <c r="O66" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P66" s="13"/>
       <c r="Q66" s="11" t="s">
@@ -6966,7 +6978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
         <v>145</v>
       </c>
@@ -7059,7 +7071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A68" s="16" t="s">
         <v>128</v>
       </c>
@@ -7152,7 +7164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A69" s="16" t="s">
         <v>146</v>
       </c>
@@ -7166,7 +7178,7 @@
         <v>29</v>
       </c>
       <c r="E69" s="34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F69" s="20"/>
       <c r="G69" s="9">
@@ -7245,7 +7257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
         <v>147</v>
       </c>
@@ -7259,7 +7271,7 @@
         <v>29</v>
       </c>
       <c r="E70" s="34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F70" s="20"/>
       <c r="G70" s="9">
@@ -7338,7 +7350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>8</v>
       </c>
@@ -7379,7 +7391,7 @@
       <c r="AJ71" s="9"/>
       <c r="AK71" s="9"/>
     </row>
-    <row r="72" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>25</v>
       </c>
@@ -7419,7 +7431,7 @@
         <v>11</v>
       </c>
       <c r="O72" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P72" s="13"/>
       <c r="Q72" s="11" t="s">
@@ -7472,7 +7484,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>134</v>
       </c>
@@ -7565,7 +7577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>129</v>
       </c>
@@ -7658,7 +7670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>148</v>
       </c>
@@ -7672,7 +7684,7 @@
         <v>29</v>
       </c>
       <c r="E75" s="34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F75" s="20"/>
       <c r="G75" s="9">
@@ -7751,7 +7763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>149</v>
       </c>
@@ -7844,7 +7856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A77" s="28" t="s">
         <v>150</v>
       </c>
@@ -7858,7 +7870,7 @@
         <v>1</v>
       </c>
       <c r="E77" s="34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F77" s="21"/>
       <c r="G77" s="9">
@@ -7886,7 +7898,7 @@
       <c r="O77" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="P77" s="38"/>
+      <c r="P77" s="42"/>
       <c r="Q77" s="35" t="s">
         <v>76</v>
       </c>
@@ -7896,34 +7908,34 @@
       <c r="S77" s="35">
         <v>1</v>
       </c>
-      <c r="T77" s="38"/>
+      <c r="T77" s="42"/>
       <c r="U77" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="V77" s="38"/>
+        <v>29</v>
+      </c>
+      <c r="V77" s="42"/>
       <c r="W77" s="35">
         <v>1</v>
       </c>
-      <c r="X77" s="38"/>
+      <c r="X77" s="42"/>
       <c r="Y77" s="35">
         <v>1</v>
       </c>
-      <c r="Z77" s="38"/>
+      <c r="Z77" s="42"/>
       <c r="AA77" s="35">
         <v>1</v>
       </c>
-      <c r="AB77" s="38"/>
+      <c r="AB77" s="42"/>
       <c r="AC77" s="35">
         <v>0</v>
       </c>
       <c r="AD77" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="AE77" s="38"/>
+      <c r="AE77" s="42"/>
       <c r="AF77" s="35">
         <v>0</v>
       </c>
-      <c r="AG77" s="38"/>
+      <c r="AG77" s="42"/>
       <c r="AH77" s="37" t="s">
         <v>137</v>
       </c>
@@ -7937,7 +7949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>151</v>
       </c>
@@ -7977,46 +7989,46 @@
         <v>27</v>
       </c>
       <c r="O78" s="35">
-        <v>1</v>
-      </c>
-      <c r="P78" s="38"/>
+        <v>10</v>
+      </c>
+      <c r="P78" s="42"/>
       <c r="Q78" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="R78" s="35" t="s">
-        <v>27</v>
+        <v>140</v>
+      </c>
+      <c r="R78" s="35">
+        <v>1101</v>
       </c>
       <c r="S78" s="35">
         <v>1</v>
       </c>
-      <c r="T78" s="38"/>
+      <c r="T78" s="42"/>
       <c r="U78" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="V78" s="38"/>
+        <v>29</v>
+      </c>
+      <c r="V78" s="42"/>
       <c r="W78" s="35">
         <v>1</v>
       </c>
-      <c r="X78" s="38"/>
+      <c r="X78" s="42"/>
       <c r="Y78" s="35">
         <v>1</v>
       </c>
-      <c r="Z78" s="38"/>
+      <c r="Z78" s="42"/>
       <c r="AA78" s="35">
         <v>1</v>
       </c>
-      <c r="AB78" s="38"/>
+      <c r="AB78" s="42"/>
       <c r="AC78" s="35">
         <v>1</v>
       </c>
       <c r="AD78" s="35">
         <v>1</v>
       </c>
-      <c r="AE78" s="38"/>
+      <c r="AE78" s="42"/>
       <c r="AF78" s="35">
         <v>0</v>
       </c>
-      <c r="AG78" s="38"/>
+      <c r="AG78" s="42"/>
       <c r="AH78" s="35" t="s">
         <v>28</v>
       </c>
@@ -8030,7 +8042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A79" s="6"/>
       <c r="B79" s="9"/>
       <c r="C79" s="34"/>
@@ -8069,7 +8081,7 @@
       <c r="AJ79" s="9"/>
       <c r="AK79" s="9"/>
     </row>
-    <row r="80" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>120</v>
       </c>
@@ -8110,34 +8122,34 @@
       <c r="AJ80" s="9"/>
       <c r="AK80" s="9"/>
     </row>
-    <row r="81" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B81" s="42" t="s">
+      <c r="B81" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="C81" s="42"/>
-      <c r="D81" s="42"/>
-      <c r="E81" s="42"/>
+      <c r="C81" s="43"/>
+      <c r="D81" s="43"/>
+      <c r="E81" s="43"/>
       <c r="F81" s="20"/>
       <c r="G81" s="20"/>
       <c r="H81" s="20"/>
-      <c r="I81" s="43" t="s">
+      <c r="I81" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="J81" s="43"/>
-      <c r="K81" s="43"/>
-      <c r="L81" s="43"/>
-      <c r="M81" s="43"/>
-      <c r="N81" s="43"/>
-      <c r="O81" s="43"/>
+      <c r="J81" s="44"/>
+      <c r="K81" s="44"/>
+      <c r="L81" s="44"/>
+      <c r="M81" s="44"/>
+      <c r="N81" s="44"/>
+      <c r="O81" s="44"/>
       <c r="P81" s="13"/>
-      <c r="Q81" s="42" t="s">
+      <c r="Q81" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="R81" s="42"/>
-      <c r="S81" s="42"/>
+      <c r="R81" s="43"/>
+      <c r="S81" s="43"/>
       <c r="T81" s="13"/>
       <c r="U81" s="7" t="s">
         <v>67</v>
@@ -8154,23 +8166,23 @@
         <v>70</v>
       </c>
       <c r="AB81" s="13"/>
-      <c r="AC81" s="43" t="s">
+      <c r="AC81" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="AD81" s="43"/>
+      <c r="AD81" s="44"/>
       <c r="AE81" s="23"/>
       <c r="AF81" s="18" t="s">
         <v>72</v>
       </c>
       <c r="AG81" s="13"/>
-      <c r="AH81" s="43" t="s">
+      <c r="AH81" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AI81" s="43"/>
-      <c r="AJ81" s="43"/>
-      <c r="AK81" s="43"/>
-    </row>
-    <row r="82" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+      <c r="AI81" s="44"/>
+      <c r="AJ81" s="44"/>
+      <c r="AK81" s="44"/>
+    </row>
+    <row r="82" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>25</v>
       </c>
@@ -8210,7 +8222,7 @@
         <v>11</v>
       </c>
       <c r="O82" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P82" s="41"/>
       <c r="Q82" s="11" t="s">
@@ -8263,9 +8275,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A83" s="16" t="s">
-        <v>121</v>
+        <v>188</v>
       </c>
       <c r="B83" s="35" t="s">
         <v>28</v>
@@ -8277,7 +8289,7 @@
         <v>29</v>
       </c>
       <c r="E83" s="34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F83" s="20"/>
       <c r="G83" s="35">
@@ -8356,9 +8368,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A84" s="16" t="s">
-        <v>125</v>
+        <v>189</v>
       </c>
       <c r="B84" s="35" t="s">
         <v>28</v>
@@ -8370,7 +8382,7 @@
         <v>29</v>
       </c>
       <c r="E84" s="34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F84" s="20"/>
       <c r="G84" s="35">
@@ -8449,7 +8461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>6</v>
       </c>
@@ -8490,7 +8502,7 @@
       <c r="AJ85" s="35"/>
       <c r="AK85" s="35"/>
     </row>
-    <row r="86" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>25</v>
       </c>
@@ -8530,7 +8542,7 @@
         <v>11</v>
       </c>
       <c r="O86" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P86" s="41"/>
       <c r="Q86" s="11" t="s">
@@ -8583,7 +8595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>152</v>
       </c>
@@ -8597,7 +8609,7 @@
         <v>29</v>
       </c>
       <c r="E87" s="34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F87" s="20"/>
       <c r="G87" s="35">
@@ -8676,7 +8688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>153</v>
       </c>
@@ -8690,7 +8702,7 @@
         <v>29</v>
       </c>
       <c r="E88" s="34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F88" s="20"/>
       <c r="G88" s="35">
@@ -8769,7 +8781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>4</v>
       </c>
@@ -8810,7 +8822,7 @@
       <c r="AJ89" s="35"/>
       <c r="AK89" s="35"/>
     </row>
-    <row r="90" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>25</v>
       </c>
@@ -8850,7 +8862,7 @@
         <v>11</v>
       </c>
       <c r="O90" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P90" s="41"/>
       <c r="Q90" s="11" t="s">
@@ -8903,7 +8915,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
         <v>154</v>
       </c>
@@ -8917,7 +8929,7 @@
         <v>29</v>
       </c>
       <c r="E91" s="34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F91" s="20"/>
       <c r="G91" s="35">
@@ -8996,7 +9008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
         <v>155</v>
       </c>
@@ -9010,7 +9022,7 @@
         <v>29</v>
       </c>
       <c r="E92" s="34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F92" s="20"/>
       <c r="G92" s="35">
@@ -9089,7 +9101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>7</v>
       </c>
@@ -9130,7 +9142,7 @@
       <c r="AJ93" s="35"/>
       <c r="AK93" s="35"/>
     </row>
-    <row r="94" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>25</v>
       </c>
@@ -9170,7 +9182,7 @@
         <v>11</v>
       </c>
       <c r="O94" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P94" s="41"/>
       <c r="Q94" s="11" t="s">
@@ -9223,7 +9235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
         <v>156</v>
       </c>
@@ -9237,7 +9249,7 @@
         <v>29</v>
       </c>
       <c r="E95" s="34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F95" s="20"/>
       <c r="G95" s="35">
@@ -9316,7 +9328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
         <v>157</v>
       </c>
@@ -9330,7 +9342,7 @@
         <v>29</v>
       </c>
       <c r="E96" s="34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F96" s="20"/>
       <c r="G96" s="35">
@@ -9409,7 +9421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>5</v>
       </c>
@@ -9450,7 +9462,7 @@
       <c r="AJ97" s="35"/>
       <c r="AK97" s="35"/>
     </row>
-    <row r="98" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>25</v>
       </c>
@@ -9490,7 +9502,7 @@
         <v>11</v>
       </c>
       <c r="O98" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P98" s="41"/>
       <c r="Q98" s="11" t="s">
@@ -9543,7 +9555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
         <v>124</v>
       </c>
@@ -9636,7 +9648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
         <v>159</v>
       </c>
@@ -9729,7 +9741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
         <v>158</v>
       </c>
@@ -9743,7 +9755,7 @@
         <v>29</v>
       </c>
       <c r="E101" s="34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F101" s="20"/>
       <c r="G101" s="35">
@@ -9822,7 +9834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
         <v>160</v>
       </c>
@@ -9836,7 +9848,7 @@
         <v>29</v>
       </c>
       <c r="E102" s="34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F102" s="20"/>
       <c r="G102" s="35">
@@ -9915,7 +9927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>8</v>
       </c>
@@ -9956,7 +9968,7 @@
       <c r="AJ103" s="35"/>
       <c r="AK103" s="35"/>
     </row>
-    <row r="104" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>25</v>
       </c>
@@ -9996,7 +10008,7 @@
         <v>11</v>
       </c>
       <c r="O104" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P104" s="41"/>
       <c r="Q104" s="11" t="s">
@@ -10049,7 +10061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
         <v>130</v>
       </c>
@@ -10142,7 +10154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
         <v>135</v>
       </c>
@@ -10235,7 +10247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
         <v>161</v>
       </c>
@@ -10249,7 +10261,7 @@
         <v>29</v>
       </c>
       <c r="E107" s="34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F107" s="20"/>
       <c r="G107" s="35">
@@ -10328,7 +10340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
         <v>162</v>
       </c>
@@ -10421,27 +10433,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:37" x14ac:dyDescent="0.55000000000000004">
-      <c r="A109" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="B109" s="35" t="s">
-        <v>21</v>
+    <row r="109" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A109" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B109" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="C109" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="D109" s="40">
-        <v>1</v>
-      </c>
-      <c r="E109" s="40" t="s">
-        <v>189</v>
-      </c>
-      <c r="F109" s="21"/>
+        <v>78</v>
+      </c>
+      <c r="D109" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="E109" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="F109" s="20"/>
       <c r="G109" s="9">
         <v>0</v>
       </c>
-      <c r="H109" s="21"/>
+      <c r="H109" s="20"/>
       <c r="I109" s="35">
         <v>1</v>
       </c>
@@ -10454,8 +10466,8 @@
       <c r="L109" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="M109" s="35" t="s">
-        <v>28</v>
+      <c r="M109" s="42">
+        <v>10</v>
       </c>
       <c r="N109" s="35" t="s">
         <v>27</v>
@@ -10464,14 +10476,14 @@
         <v>28</v>
       </c>
       <c r="P109" s="38"/>
-      <c r="Q109" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="R109" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="S109" s="35">
-        <v>1</v>
+      <c r="Q109" s="35">
+        <v>0</v>
+      </c>
+      <c r="R109" s="35">
+        <v>1101</v>
+      </c>
+      <c r="S109" s="35" t="s">
+        <v>29</v>
       </c>
       <c r="T109" s="38"/>
       <c r="U109" s="35" t="s">
@@ -10490,11 +10502,11 @@
         <v>1</v>
       </c>
       <c r="AB109" s="38"/>
-      <c r="AC109" s="35">
-        <v>0</v>
-      </c>
-      <c r="AD109" s="35" t="s">
-        <v>29</v>
+      <c r="AC109" s="42">
+        <v>0</v>
+      </c>
+      <c r="AD109" s="42">
+        <v>0</v>
       </c>
       <c r="AE109" s="38"/>
       <c r="AF109" s="35">
@@ -10508,33 +10520,33 @@
         <v>28</v>
       </c>
       <c r="AJ109" s="35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK109" s="35">
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:37" x14ac:dyDescent="0.55000000000000004">
-      <c r="A110" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="B110" s="9" t="s">
-        <v>28</v>
+    <row r="110" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A110" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="B110" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C110" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="D110" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="E110" s="34" t="s">
-        <v>122</v>
-      </c>
-      <c r="F110" s="20"/>
+        <v>59</v>
+      </c>
+      <c r="D110" s="40">
+        <v>1</v>
+      </c>
+      <c r="E110" s="40" t="s">
+        <v>185</v>
+      </c>
+      <c r="F110" s="21"/>
       <c r="G110" s="9">
         <v>0</v>
       </c>
-      <c r="H110" s="20"/>
+      <c r="H110" s="21"/>
       <c r="I110" s="35">
         <v>1</v>
       </c>
@@ -10563,8 +10575,8 @@
       <c r="R110" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="S110" s="35" t="s">
-        <v>29</v>
+      <c r="S110" s="35">
+        <v>1</v>
       </c>
       <c r="T110" s="38"/>
       <c r="U110" s="35" t="s">
@@ -10601,52 +10613,16 @@
         <v>28</v>
       </c>
       <c r="AJ110" s="35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK110" s="35">
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:37" x14ac:dyDescent="0.55000000000000004">
-      <c r="A111" s="6"/>
-      <c r="B111" s="9"/>
-      <c r="C111" s="40"/>
-      <c r="D111" s="9"/>
-      <c r="E111" s="40"/>
-      <c r="F111" s="20"/>
-      <c r="G111" s="9"/>
-      <c r="H111" s="20"/>
-      <c r="I111" s="9"/>
-      <c r="J111" s="9"/>
-      <c r="K111" s="9"/>
-      <c r="L111" s="9"/>
-      <c r="M111" s="9"/>
-      <c r="N111" s="9"/>
-      <c r="O111" s="9"/>
-      <c r="P111" s="13"/>
-      <c r="Q111" s="9"/>
-      <c r="R111" s="9"/>
-      <c r="S111" s="9"/>
-      <c r="T111" s="13"/>
-      <c r="U111" s="9"/>
-      <c r="V111" s="13"/>
-      <c r="W111" s="9"/>
-      <c r="X111" s="13"/>
-      <c r="Y111" s="9"/>
-      <c r="Z111" s="13"/>
-      <c r="AA111" s="9"/>
-      <c r="AB111" s="13"/>
-      <c r="AC111" s="9"/>
-      <c r="AD111" s="9"/>
-      <c r="AE111" s="13"/>
-      <c r="AF111" s="9"/>
-      <c r="AG111" s="13"/>
-      <c r="AH111" s="9"/>
-      <c r="AI111" s="9"/>
-      <c r="AJ111" s="9"/>
-      <c r="AK111" s="9"/>
-    </row>
-    <row r="112" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A111" s="47"/>
+    </row>
+    <row r="112" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>39</v>
       </c>
@@ -10687,34 +10663,34 @@
       <c r="AJ112" s="9"/>
       <c r="AK112" s="9"/>
     </row>
-    <row r="113" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B113" s="42" t="s">
+      <c r="B113" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="C113" s="42"/>
-      <c r="D113" s="42"/>
-      <c r="E113" s="42"/>
+      <c r="C113" s="43"/>
+      <c r="D113" s="43"/>
+      <c r="E113" s="43"/>
       <c r="F113" s="20"/>
       <c r="G113" s="20"/>
       <c r="H113" s="20"/>
-      <c r="I113" s="43" t="s">
+      <c r="I113" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="J113" s="43"/>
-      <c r="K113" s="43"/>
-      <c r="L113" s="43"/>
-      <c r="M113" s="43"/>
-      <c r="N113" s="43"/>
-      <c r="O113" s="43"/>
+      <c r="J113" s="44"/>
+      <c r="K113" s="44"/>
+      <c r="L113" s="44"/>
+      <c r="M113" s="44"/>
+      <c r="N113" s="44"/>
+      <c r="O113" s="44"/>
       <c r="P113" s="13"/>
-      <c r="Q113" s="42" t="s">
+      <c r="Q113" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="R113" s="42"/>
-      <c r="S113" s="42"/>
+      <c r="R113" s="43"/>
+      <c r="S113" s="43"/>
       <c r="T113" s="13"/>
       <c r="U113" s="7" t="s">
         <v>67</v>
@@ -10731,23 +10707,23 @@
         <v>70</v>
       </c>
       <c r="AB113" s="13"/>
-      <c r="AC113" s="43" t="s">
+      <c r="AC113" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="AD113" s="43"/>
+      <c r="AD113" s="44"/>
       <c r="AE113" s="23"/>
       <c r="AF113" s="18" t="s">
         <v>72</v>
       </c>
       <c r="AG113" s="13"/>
-      <c r="AH113" s="43" t="s">
+      <c r="AH113" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AI113" s="43"/>
-      <c r="AJ113" s="43"/>
-      <c r="AK113" s="43"/>
-    </row>
-    <row r="114" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+      <c r="AI113" s="44"/>
+      <c r="AJ113" s="44"/>
+      <c r="AK113" s="44"/>
+    </row>
+    <row r="114" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>25</v>
       </c>
@@ -10787,7 +10763,7 @@
         <v>11</v>
       </c>
       <c r="O114" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P114" s="13"/>
       <c r="Q114" s="11" t="s">
@@ -10840,9 +10816,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B115" s="9" t="s">
         <v>28</v>
@@ -10933,9 +10909,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B116" s="9" t="s">
         <v>28</v>
@@ -11026,7 +11002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>4</v>
       </c>
@@ -11067,7 +11043,7 @@
       <c r="AJ117" s="9"/>
       <c r="AK117" s="9"/>
     </row>
-    <row r="118" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>25</v>
       </c>
@@ -11107,7 +11083,7 @@
         <v>11</v>
       </c>
       <c r="O118" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P118" s="13"/>
       <c r="Q118" s="11" t="s">
@@ -11160,9 +11136,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B119" s="9" t="s">
         <v>28</v>
@@ -11253,9 +11229,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B120" s="9" t="s">
         <v>28</v>
@@ -11346,7 +11322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>5</v>
       </c>
@@ -11387,7 +11363,7 @@
       <c r="AJ121" s="9"/>
       <c r="AK121" s="9"/>
     </row>
-    <row r="122" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>25</v>
       </c>
@@ -11427,7 +11403,7 @@
         <v>11</v>
       </c>
       <c r="O122" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P122" s="13"/>
       <c r="Q122" s="11" t="s">
@@ -11480,9 +11456,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B123" s="9" t="s">
         <v>28</v>
@@ -11573,9 +11549,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B124" s="9" t="s">
         <v>28</v>
@@ -11666,9 +11642,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B125" s="9" t="s">
         <v>28</v>
@@ -11759,9 +11735,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B126" s="9" t="s">
         <v>28</v>
@@ -11852,9 +11828,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A127" s="28" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B127" s="9" t="s">
         <v>21</v>
@@ -11945,9 +11921,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B128" s="9" t="s">
         <v>28</v>
@@ -12038,7 +12014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A129" s="6"/>
       <c r="B129" s="9"/>
       <c r="C129" s="40"/>
@@ -12077,7 +12053,7 @@
       <c r="AJ129" s="9"/>
       <c r="AK129" s="9"/>
     </row>
-    <row r="130" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>40</v>
       </c>
@@ -12118,34 +12094,34 @@
       <c r="AJ130" s="9"/>
       <c r="AK130" s="9"/>
     </row>
-    <row r="131" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B131" s="42" t="s">
+      <c r="B131" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="C131" s="42"/>
-      <c r="D131" s="42"/>
-      <c r="E131" s="42"/>
+      <c r="C131" s="43"/>
+      <c r="D131" s="43"/>
+      <c r="E131" s="43"/>
       <c r="F131" s="20"/>
       <c r="G131" s="20"/>
       <c r="H131" s="20"/>
-      <c r="I131" s="43" t="s">
+      <c r="I131" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="J131" s="43"/>
-      <c r="K131" s="43"/>
-      <c r="L131" s="43"/>
-      <c r="M131" s="43"/>
-      <c r="N131" s="43"/>
-      <c r="O131" s="43"/>
+      <c r="J131" s="44"/>
+      <c r="K131" s="44"/>
+      <c r="L131" s="44"/>
+      <c r="M131" s="44"/>
+      <c r="N131" s="44"/>
+      <c r="O131" s="44"/>
       <c r="P131" s="13"/>
-      <c r="Q131" s="42" t="s">
+      <c r="Q131" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="R131" s="42"/>
-      <c r="S131" s="42"/>
+      <c r="R131" s="43"/>
+      <c r="S131" s="43"/>
       <c r="T131" s="13"/>
       <c r="U131" s="7" t="s">
         <v>67</v>
@@ -12162,23 +12138,23 @@
         <v>70</v>
       </c>
       <c r="AB131" s="13"/>
-      <c r="AC131" s="43" t="s">
+      <c r="AC131" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="AD131" s="43"/>
+      <c r="AD131" s="44"/>
       <c r="AE131" s="23"/>
       <c r="AF131" s="18" t="s">
         <v>72</v>
       </c>
       <c r="AG131" s="13"/>
-      <c r="AH131" s="43" t="s">
+      <c r="AH131" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AI131" s="43"/>
-      <c r="AJ131" s="43"/>
-      <c r="AK131" s="43"/>
-    </row>
-    <row r="132" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+      <c r="AI131" s="44"/>
+      <c r="AJ131" s="44"/>
+      <c r="AK131" s="44"/>
+    </row>
+    <row r="132" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>25</v>
       </c>
@@ -12218,7 +12194,7 @@
         <v>11</v>
       </c>
       <c r="O132" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P132" s="13"/>
       <c r="Q132" s="11" t="s">
@@ -12271,9 +12247,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B133" s="9" t="s">
         <v>28</v>
@@ -12285,7 +12261,7 @@
         <v>29</v>
       </c>
       <c r="E133" s="40" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F133" s="20"/>
       <c r="G133" s="9">
@@ -12364,9 +12340,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B134" s="9" t="s">
         <v>28</v>
@@ -12378,7 +12354,7 @@
         <v>29</v>
       </c>
       <c r="E134" s="40" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F134" s="20"/>
       <c r="G134" s="9">
@@ -12457,7 +12433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>4</v>
       </c>
@@ -12498,7 +12474,7 @@
       <c r="AJ135" s="9"/>
       <c r="AK135" s="9"/>
     </row>
-    <row r="136" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>25</v>
       </c>
@@ -12538,7 +12514,7 @@
         <v>11</v>
       </c>
       <c r="O136" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P136" s="13"/>
       <c r="Q136" s="11" t="s">
@@ -12591,9 +12567,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A137" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B137" s="9" t="s">
         <v>28</v>
@@ -12605,7 +12581,7 @@
         <v>29</v>
       </c>
       <c r="E137" s="40" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F137" s="20"/>
       <c r="G137" s="9">
@@ -12684,9 +12660,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A138" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B138" s="9" t="s">
         <v>28</v>
@@ -12698,7 +12674,7 @@
         <v>29</v>
       </c>
       <c r="E138" s="40" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F138" s="20"/>
       <c r="G138" s="9">
@@ -12777,7 +12753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>5</v>
       </c>
@@ -12818,7 +12794,7 @@
       <c r="AJ139" s="9"/>
       <c r="AK139" s="9"/>
     </row>
-    <row r="140" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>25</v>
       </c>
@@ -12858,7 +12834,7 @@
         <v>11</v>
       </c>
       <c r="O140" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P140" s="13"/>
       <c r="Q140" s="11" t="s">
@@ -12911,9 +12887,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B141" s="9" t="s">
         <v>28</v>
@@ -13004,9 +12980,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B142" s="9" t="s">
         <v>28</v>
@@ -13097,9 +13073,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A143" s="6" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B143" s="9" t="s">
         <v>28</v>
@@ -13111,7 +13087,7 @@
         <v>29</v>
       </c>
       <c r="E143" s="40" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F143" s="20"/>
       <c r="G143" s="9">
@@ -13190,9 +13166,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A144" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B144" s="9" t="s">
         <v>28</v>
@@ -13283,193 +13259,193 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:37" x14ac:dyDescent="0.55000000000000004">
-      <c r="A145" s="28" t="s">
-        <v>179</v>
-      </c>
-      <c r="B145" s="9" t="s">
+    <row r="145" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A145" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B145" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C145" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="D145" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="E145" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="F145" s="20"/>
+      <c r="G145" s="35">
+        <v>0</v>
+      </c>
+      <c r="H145" s="20"/>
+      <c r="I145" s="35">
+        <v>1</v>
+      </c>
+      <c r="J145" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="K145" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="L145" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="M145" s="42">
+        <v>10</v>
+      </c>
+      <c r="N145" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="O145" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="P145" s="42"/>
+      <c r="Q145" s="35">
+        <v>0</v>
+      </c>
+      <c r="R145" s="35">
+        <v>1101</v>
+      </c>
+      <c r="S145" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="T145" s="42"/>
+      <c r="U145" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="V145" s="42"/>
+      <c r="W145" s="35">
+        <v>1</v>
+      </c>
+      <c r="X145" s="42"/>
+      <c r="Y145" s="35">
+        <v>1</v>
+      </c>
+      <c r="Z145" s="42"/>
+      <c r="AA145" s="35">
+        <v>1</v>
+      </c>
+      <c r="AB145" s="42"/>
+      <c r="AC145" s="42">
+        <v>0</v>
+      </c>
+      <c r="AD145" s="42">
+        <v>0</v>
+      </c>
+      <c r="AE145" s="42"/>
+      <c r="AF145" s="35">
+        <v>0</v>
+      </c>
+      <c r="AG145" s="42"/>
+      <c r="AH145" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="AI145" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ145" s="35">
+        <v>0</v>
+      </c>
+      <c r="AK145" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A146" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="B146" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C145" s="34" t="s">
+      <c r="C146" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="D145" s="40">
-        <v>1</v>
-      </c>
-      <c r="E145" s="40" t="s">
-        <v>190</v>
-      </c>
-      <c r="F145" s="21"/>
-      <c r="G145" s="9">
-        <v>0</v>
-      </c>
-      <c r="H145" s="21"/>
-      <c r="I145" s="9">
-        <v>1</v>
-      </c>
-      <c r="J145" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="K145" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L145" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="M145" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="N145" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="O145" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="P145" s="13"/>
-      <c r="Q145" s="9" t="s">
+      <c r="D146" s="42">
+        <v>1</v>
+      </c>
+      <c r="E146" s="42" t="s">
+        <v>185</v>
+      </c>
+      <c r="F146" s="21"/>
+      <c r="G146" s="35">
+        <v>0</v>
+      </c>
+      <c r="H146" s="21"/>
+      <c r="I146" s="35">
+        <v>1</v>
+      </c>
+      <c r="J146" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="K146" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="L146" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="M146" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="N146" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="O146" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="P146" s="42"/>
+      <c r="Q146" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="R145" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="S145" s="9">
-        <v>1</v>
-      </c>
-      <c r="T145" s="13"/>
-      <c r="U145" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="V145" s="13"/>
-      <c r="W145" s="9">
-        <v>1</v>
-      </c>
-      <c r="X145" s="13"/>
-      <c r="Y145" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z145" s="13"/>
-      <c r="AA145" s="9">
-        <v>1</v>
-      </c>
-      <c r="AB145" s="13"/>
-      <c r="AC145" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD145" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE145" s="13"/>
-      <c r="AF145" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG145" s="13"/>
-      <c r="AH145" s="17" t="s">
+      <c r="R146" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="S146" s="35">
+        <v>1</v>
+      </c>
+      <c r="T146" s="42"/>
+      <c r="U146" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="V146" s="42"/>
+      <c r="W146" s="35">
+        <v>1</v>
+      </c>
+      <c r="X146" s="42"/>
+      <c r="Y146" s="35">
+        <v>1</v>
+      </c>
+      <c r="Z146" s="42"/>
+      <c r="AA146" s="35">
+        <v>1</v>
+      </c>
+      <c r="AB146" s="42"/>
+      <c r="AC146" s="35">
+        <v>1</v>
+      </c>
+      <c r="AD146" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE146" s="42"/>
+      <c r="AF146" s="35">
+        <v>0</v>
+      </c>
+      <c r="AG146" s="42"/>
+      <c r="AH146" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="AI145" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="AJ145" s="9">
-        <v>1</v>
-      </c>
-      <c r="AK145" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="1:37" x14ac:dyDescent="0.55000000000000004">
-      <c r="A146" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="B146" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C146" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="D146" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="E146" s="34" t="s">
-        <v>122</v>
-      </c>
-      <c r="F146" s="20"/>
-      <c r="G146" s="9">
-        <v>0</v>
-      </c>
-      <c r="H146" s="20"/>
-      <c r="I146" s="9">
-        <v>1</v>
-      </c>
-      <c r="J146" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="K146" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L146" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="M146" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="N146" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="O146" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="P146" s="13"/>
-      <c r="Q146" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="R146" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="S146" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="T146" s="13"/>
-      <c r="U146" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="V146" s="13"/>
-      <c r="W146" s="9">
-        <v>1</v>
-      </c>
-      <c r="X146" s="13"/>
-      <c r="Y146" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z146" s="13"/>
-      <c r="AA146" s="9">
-        <v>1</v>
-      </c>
-      <c r="AB146" s="13"/>
-      <c r="AC146" s="9">
-        <v>1</v>
-      </c>
-      <c r="AD146" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE146" s="13"/>
-      <c r="AF146" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG146" s="13"/>
-      <c r="AH146" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="AI146" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="AJ146" s="9">
-        <v>0</v>
-      </c>
-      <c r="AK146" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+      <c r="AI146" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ146" s="35">
+        <v>1</v>
+      </c>
+      <c r="AK146" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A147" s="6"/>
       <c r="B147" s="9"/>
       <c r="C147" s="40"/>
@@ -13508,34 +13484,34 @@
       <c r="AJ147" s="9"/>
       <c r="AK147" s="9"/>
     </row>
-    <row r="148" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B148" s="42" t="s">
+      <c r="B148" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="C148" s="42"/>
-      <c r="D148" s="42"/>
-      <c r="E148" s="42"/>
+      <c r="C148" s="43"/>
+      <c r="D148" s="43"/>
+      <c r="E148" s="43"/>
       <c r="F148" s="20"/>
       <c r="G148" s="20"/>
       <c r="H148" s="20"/>
-      <c r="I148" s="43" t="s">
+      <c r="I148" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="J148" s="43"/>
-      <c r="K148" s="43"/>
-      <c r="L148" s="43"/>
-      <c r="M148" s="43"/>
-      <c r="N148" s="43"/>
-      <c r="O148" s="43"/>
+      <c r="J148" s="44"/>
+      <c r="K148" s="44"/>
+      <c r="L148" s="44"/>
+      <c r="M148" s="44"/>
+      <c r="N148" s="44"/>
+      <c r="O148" s="44"/>
       <c r="P148" s="13"/>
-      <c r="Q148" s="42" t="s">
+      <c r="Q148" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="R148" s="42"/>
-      <c r="S148" s="42"/>
+      <c r="R148" s="43"/>
+      <c r="S148" s="43"/>
       <c r="T148" s="13"/>
       <c r="U148" s="7" t="s">
         <v>67</v>
@@ -13552,23 +13528,23 @@
         <v>70</v>
       </c>
       <c r="AB148" s="13"/>
-      <c r="AC148" s="43" t="s">
+      <c r="AC148" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="AD148" s="43"/>
+      <c r="AD148" s="44"/>
       <c r="AE148" s="23"/>
       <c r="AF148" s="18" t="s">
         <v>72</v>
       </c>
       <c r="AG148" s="13"/>
-      <c r="AH148" s="43" t="s">
+      <c r="AH148" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AI148" s="43"/>
-      <c r="AJ148" s="43"/>
-      <c r="AK148" s="43"/>
-    </row>
-    <row r="149" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+      <c r="AI148" s="44"/>
+      <c r="AJ148" s="44"/>
+      <c r="AK148" s="44"/>
+    </row>
+    <row r="149" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>25</v>
       </c>
@@ -13608,7 +13584,7 @@
         <v>11</v>
       </c>
       <c r="O149" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P149" s="13"/>
       <c r="Q149" s="11" t="s">
@@ -13661,7 +13637,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A150" s="6">
         <v>92</v>
       </c>
@@ -13754,7 +13730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A151" s="6"/>
       <c r="B151" s="9"/>
       <c r="C151" s="40"/>
@@ -13793,34 +13769,34 @@
       <c r="AJ151" s="9"/>
       <c r="AK151" s="9"/>
     </row>
-    <row r="152" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B152" s="42" t="s">
+      <c r="B152" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="C152" s="42"/>
-      <c r="D152" s="42"/>
-      <c r="E152" s="42"/>
+      <c r="C152" s="43"/>
+      <c r="D152" s="43"/>
+      <c r="E152" s="43"/>
       <c r="F152" s="20"/>
       <c r="G152" s="20"/>
       <c r="H152" s="20"/>
-      <c r="I152" s="43" t="s">
+      <c r="I152" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="J152" s="43"/>
-      <c r="K152" s="43"/>
-      <c r="L152" s="43"/>
-      <c r="M152" s="43"/>
-      <c r="N152" s="43"/>
-      <c r="O152" s="43"/>
+      <c r="J152" s="44"/>
+      <c r="K152" s="44"/>
+      <c r="L152" s="44"/>
+      <c r="M152" s="44"/>
+      <c r="N152" s="44"/>
+      <c r="O152" s="44"/>
       <c r="P152" s="13"/>
-      <c r="Q152" s="42" t="s">
+      <c r="Q152" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="R152" s="42"/>
-      <c r="S152" s="42"/>
+      <c r="R152" s="43"/>
+      <c r="S152" s="43"/>
       <c r="T152" s="13"/>
       <c r="U152" s="7" t="s">
         <v>67</v>
@@ -13837,23 +13813,23 @@
         <v>70</v>
       </c>
       <c r="AB152" s="13"/>
-      <c r="AC152" s="43" t="s">
+      <c r="AC152" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="AD152" s="43"/>
+      <c r="AD152" s="44"/>
       <c r="AE152" s="23"/>
       <c r="AF152" s="18" t="s">
         <v>72</v>
       </c>
       <c r="AG152" s="13"/>
-      <c r="AH152" s="43" t="s">
+      <c r="AH152" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AI152" s="43"/>
-      <c r="AJ152" s="43"/>
-      <c r="AK152" s="43"/>
-    </row>
-    <row r="153" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+      <c r="AI152" s="44"/>
+      <c r="AJ152" s="44"/>
+      <c r="AK152" s="44"/>
+    </row>
+    <row r="153" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>25</v>
       </c>
@@ -13893,7 +13869,7 @@
         <v>11</v>
       </c>
       <c r="O153" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P153" s="13"/>
       <c r="Q153" s="11" t="s">
@@ -13946,7 +13922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="154" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A154" s="6">
         <v>93</v>
       </c>
@@ -14039,7 +14015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B155" s="9"/>
       <c r="C155" s="40"/>
       <c r="D155" s="9"/>
@@ -14077,34 +14053,34 @@
       <c r="AJ155" s="9"/>
       <c r="AK155" s="9"/>
     </row>
-    <row r="156" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B156" s="42" t="s">
+      <c r="B156" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="C156" s="42"/>
-      <c r="D156" s="42"/>
-      <c r="E156" s="42"/>
+      <c r="C156" s="43"/>
+      <c r="D156" s="43"/>
+      <c r="E156" s="43"/>
       <c r="F156" s="20"/>
       <c r="G156" s="20"/>
       <c r="H156" s="20"/>
-      <c r="I156" s="43" t="s">
+      <c r="I156" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="J156" s="43"/>
-      <c r="K156" s="43"/>
-      <c r="L156" s="43"/>
-      <c r="M156" s="43"/>
-      <c r="N156" s="43"/>
-      <c r="O156" s="43"/>
+      <c r="J156" s="44"/>
+      <c r="K156" s="44"/>
+      <c r="L156" s="44"/>
+      <c r="M156" s="44"/>
+      <c r="N156" s="44"/>
+      <c r="O156" s="44"/>
       <c r="P156" s="13"/>
-      <c r="Q156" s="42" t="s">
+      <c r="Q156" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="R156" s="42"/>
-      <c r="S156" s="42"/>
+      <c r="R156" s="43"/>
+      <c r="S156" s="43"/>
       <c r="T156" s="13"/>
       <c r="U156" s="7" t="s">
         <v>67</v>
@@ -14121,23 +14097,23 @@
         <v>70</v>
       </c>
       <c r="AB156" s="13"/>
-      <c r="AC156" s="43" t="s">
+      <c r="AC156" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="AD156" s="43"/>
+      <c r="AD156" s="44"/>
       <c r="AE156" s="23"/>
       <c r="AF156" s="18" t="s">
         <v>72</v>
       </c>
       <c r="AG156" s="13"/>
-      <c r="AH156" s="43" t="s">
+      <c r="AH156" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AI156" s="43"/>
-      <c r="AJ156" s="43"/>
-      <c r="AK156" s="43"/>
-    </row>
-    <row r="157" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+      <c r="AI156" s="44"/>
+      <c r="AJ156" s="44"/>
+      <c r="AK156" s="44"/>
+    </row>
+    <row r="157" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>25</v>
       </c>
@@ -14177,7 +14153,7 @@
         <v>11</v>
       </c>
       <c r="O157" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P157" s="13"/>
       <c r="Q157" s="11" t="s">
@@ -14230,7 +14206,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="158" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A158" s="27">
         <v>94</v>
       </c>
@@ -14275,7 +14251,7 @@
       <c r="AJ158" s="25"/>
       <c r="AK158" s="25"/>
     </row>
-    <row r="159" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A159" s="6"/>
       <c r="B159" s="9"/>
       <c r="C159" s="40"/>
@@ -14314,34 +14290,34 @@
       <c r="AJ159" s="9"/>
       <c r="AK159" s="9"/>
     </row>
-    <row r="160" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B160" s="42" t="s">
+      <c r="B160" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="C160" s="42"/>
-      <c r="D160" s="42"/>
-      <c r="E160" s="42"/>
+      <c r="C160" s="43"/>
+      <c r="D160" s="43"/>
+      <c r="E160" s="43"/>
       <c r="F160" s="20"/>
       <c r="G160" s="20"/>
       <c r="H160" s="20"/>
-      <c r="I160" s="43" t="s">
+      <c r="I160" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="J160" s="43"/>
-      <c r="K160" s="43"/>
-      <c r="L160" s="43"/>
-      <c r="M160" s="43"/>
-      <c r="N160" s="43"/>
-      <c r="O160" s="43"/>
+      <c r="J160" s="44"/>
+      <c r="K160" s="44"/>
+      <c r="L160" s="44"/>
+      <c r="M160" s="44"/>
+      <c r="N160" s="44"/>
+      <c r="O160" s="44"/>
       <c r="P160" s="13"/>
-      <c r="Q160" s="42" t="s">
+      <c r="Q160" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="R160" s="42"/>
-      <c r="S160" s="42"/>
+      <c r="R160" s="43"/>
+      <c r="S160" s="43"/>
       <c r="T160" s="13"/>
       <c r="U160" s="7" t="s">
         <v>67</v>
@@ -14358,23 +14334,23 @@
         <v>70</v>
       </c>
       <c r="AB160" s="13"/>
-      <c r="AC160" s="43" t="s">
+      <c r="AC160" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="AD160" s="43"/>
+      <c r="AD160" s="44"/>
       <c r="AE160" s="23"/>
       <c r="AF160" s="18" t="s">
         <v>72</v>
       </c>
       <c r="AG160" s="13"/>
-      <c r="AH160" s="43" t="s">
+      <c r="AH160" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AI160" s="43"/>
-      <c r="AJ160" s="43"/>
-      <c r="AK160" s="43"/>
-    </row>
-    <row r="161" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+      <c r="AI160" s="44"/>
+      <c r="AJ160" s="44"/>
+      <c r="AK160" s="44"/>
+    </row>
+    <row r="161" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>25</v>
       </c>
@@ -14414,7 +14390,7 @@
         <v>11</v>
       </c>
       <c r="O161" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P161" s="13"/>
       <c r="Q161" s="11" t="s">
@@ -14467,7 +14443,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A162" s="27">
         <v>95</v>
       </c>
@@ -14512,7 +14488,7 @@
       <c r="AJ162" s="25"/>
       <c r="AK162" s="25"/>
     </row>
-    <row r="163" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A163" s="6"/>
       <c r="B163" s="9"/>
       <c r="C163" s="40"/>
@@ -14552,167 +14528,179 @@
       <c r="AK163" s="9"/>
       <c r="AL163" s="8"/>
     </row>
-    <row r="164" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:38" x14ac:dyDescent="0.25">
       <c r="AL164" s="8"/>
     </row>
-    <row r="165" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:38" x14ac:dyDescent="0.25">
       <c r="AL165" s="8"/>
     </row>
-    <row r="166" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:38" x14ac:dyDescent="0.25">
       <c r="AL166" s="8"/>
     </row>
-    <row r="167" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A167" s="39"/>
       <c r="AL167" s="8"/>
     </row>
-    <row r="168" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:38" x14ac:dyDescent="0.25">
       <c r="AL168" s="8"/>
     </row>
-    <row r="169" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:38" x14ac:dyDescent="0.25">
       <c r="AL169" s="8"/>
     </row>
-    <row r="170" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:38" x14ac:dyDescent="0.25">
       <c r="AL170" s="8"/>
     </row>
-    <row r="171" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:38" x14ac:dyDescent="0.25">
       <c r="AL171" s="8"/>
     </row>
-    <row r="172" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:38" x14ac:dyDescent="0.25">
       <c r="AL172" s="8"/>
     </row>
-    <row r="173" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:38" x14ac:dyDescent="0.25">
       <c r="AL173" s="8"/>
     </row>
-    <row r="174" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:38" x14ac:dyDescent="0.25">
       <c r="AL174" s="8"/>
     </row>
-    <row r="175" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:38" x14ac:dyDescent="0.25">
       <c r="AL175" s="8"/>
     </row>
-    <row r="176" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:38" x14ac:dyDescent="0.25">
       <c r="AL176" s="8"/>
     </row>
-    <row r="177" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL177" s="8"/>
     </row>
-    <row r="178" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL178" s="8"/>
     </row>
-    <row r="179" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL179" s="8"/>
     </row>
-    <row r="180" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL180" s="8"/>
     </row>
-    <row r="181" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL181" s="8"/>
     </row>
-    <row r="182" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL182" s="8"/>
     </row>
-    <row r="183" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL183" s="8"/>
     </row>
-    <row r="184" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL184" s="8"/>
     </row>
-    <row r="185" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL185" s="8"/>
     </row>
-    <row r="186" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL186" s="8"/>
     </row>
-    <row r="187" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL187" s="8"/>
     </row>
-    <row r="188" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL188" s="8"/>
     </row>
-    <row r="189" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL189" s="8"/>
     </row>
-    <row r="190" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL190" s="8"/>
     </row>
-    <row r="191" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL191" s="8"/>
     </row>
-    <row r="192" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL192" s="8"/>
     </row>
-    <row r="193" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL193" s="8"/>
     </row>
-    <row r="194" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL194" s="8"/>
     </row>
-    <row r="195" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL195" s="8"/>
     </row>
-    <row r="196" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL196" s="8"/>
     </row>
-    <row r="197" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL197" s="8"/>
     </row>
-    <row r="198" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL198" s="8"/>
     </row>
-    <row r="199" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL199" s="8"/>
     </row>
-    <row r="200" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL200" s="8"/>
     </row>
-    <row r="201" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL201" s="8"/>
     </row>
-    <row r="202" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL202" s="8"/>
     </row>
-    <row r="203" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL203" s="8"/>
     </row>
-    <row r="204" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL204" s="8"/>
     </row>
-    <row r="205" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL205" s="8"/>
     </row>
-    <row r="206" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL206" s="8"/>
     </row>
-    <row r="207" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL207" s="8"/>
     </row>
-    <row r="208" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL208" s="8"/>
     </row>
-    <row r="209" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL209" s="8"/>
     </row>
-    <row r="210" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL210" s="8"/>
     </row>
-    <row r="211" spans="38:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="38:38" x14ac:dyDescent="0.25">
       <c r="AL211" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="B148:E148"/>
-    <mergeCell ref="B152:E152"/>
-    <mergeCell ref="I81:O81"/>
-    <mergeCell ref="I113:O113"/>
-    <mergeCell ref="I131:O131"/>
-    <mergeCell ref="Q81:S81"/>
-    <mergeCell ref="Q113:S113"/>
-    <mergeCell ref="Q131:S131"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="I11:N11"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="I12:O12"/>
+    <mergeCell ref="B160:E160"/>
+    <mergeCell ref="AC160:AD160"/>
+    <mergeCell ref="AH160:AK160"/>
+    <mergeCell ref="I160:O160"/>
+    <mergeCell ref="Q160:S160"/>
+    <mergeCell ref="B156:E156"/>
+    <mergeCell ref="AC156:AD156"/>
+    <mergeCell ref="AH156:AK156"/>
+    <mergeCell ref="I156:O156"/>
+    <mergeCell ref="Q156:S156"/>
+    <mergeCell ref="AH12:AK12"/>
+    <mergeCell ref="AH49:AK49"/>
+    <mergeCell ref="AI11:AK11"/>
+    <mergeCell ref="AC113:AD113"/>
+    <mergeCell ref="Q148:S148"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="Q49:S49"/>
+    <mergeCell ref="AC12:AD12"/>
+    <mergeCell ref="AH131:AK131"/>
+    <mergeCell ref="AC131:AD131"/>
+    <mergeCell ref="AC81:AD81"/>
+    <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="AC11:AD11"/>
     <mergeCell ref="AC152:AD152"/>
     <mergeCell ref="D47:AI47"/>
     <mergeCell ref="AC49:AD49"/>
@@ -14729,32 +14717,20 @@
     <mergeCell ref="AH81:AK81"/>
     <mergeCell ref="B113:E113"/>
     <mergeCell ref="AH113:AK113"/>
-    <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="AC11:AD11"/>
-    <mergeCell ref="AH12:AK12"/>
-    <mergeCell ref="AH49:AK49"/>
-    <mergeCell ref="AI11:AK11"/>
-    <mergeCell ref="AC113:AD113"/>
-    <mergeCell ref="Q148:S148"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="Q49:S49"/>
-    <mergeCell ref="AC12:AD12"/>
-    <mergeCell ref="AH131:AK131"/>
-    <mergeCell ref="AC131:AD131"/>
-    <mergeCell ref="AC81:AD81"/>
-    <mergeCell ref="B156:E156"/>
-    <mergeCell ref="AC156:AD156"/>
-    <mergeCell ref="AH156:AK156"/>
-    <mergeCell ref="I156:O156"/>
-    <mergeCell ref="Q156:S156"/>
-    <mergeCell ref="B160:E160"/>
-    <mergeCell ref="AC160:AD160"/>
-    <mergeCell ref="AH160:AK160"/>
-    <mergeCell ref="I160:O160"/>
-    <mergeCell ref="Q160:S160"/>
+    <mergeCell ref="Q81:S81"/>
+    <mergeCell ref="Q113:S113"/>
+    <mergeCell ref="Q131:S131"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="I11:N11"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="I12:O12"/>
+    <mergeCell ref="B148:E148"/>
+    <mergeCell ref="B152:E152"/>
+    <mergeCell ref="I81:O81"/>
+    <mergeCell ref="I113:O113"/>
+    <mergeCell ref="I131:O131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="44" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Phase 3 presentation data
</commit_message>
<xml_diff>
--- a/ArquiProjecto/Phase2/ControlStateDiagram.xlsx
+++ b/ArquiProjecto/Phase2/ControlStateDiagram.xlsx
@@ -1227,6 +1227,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1238,9 +1241,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1527,8 +1527,8 @@
   </sheetPr>
   <dimension ref="A1:AQ211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E141" sqref="E141"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,30 +1565,30 @@
       <c r="A2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
-      <c r="I2" s="45" t="s">
+      <c r="I2" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
       <c r="P2" s="13"/>
-      <c r="Q2" s="44" t="s">
+      <c r="Q2" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="R2" s="44"/>
-      <c r="S2" s="44"/>
+      <c r="R2" s="45"/>
+      <c r="S2" s="45"/>
       <c r="T2" s="13"/>
       <c r="U2" s="7" t="s">
         <v>65</v>
@@ -1605,21 +1605,21 @@
         <v>68</v>
       </c>
       <c r="AB2" s="13"/>
-      <c r="AC2" s="45" t="s">
+      <c r="AC2" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="AD2" s="45"/>
+      <c r="AD2" s="46"/>
       <c r="AE2" s="23"/>
       <c r="AF2" s="18" t="s">
         <v>70</v>
       </c>
       <c r="AG2" s="13"/>
-      <c r="AH2" s="45" t="s">
+      <c r="AH2" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="AI2" s="45"/>
-      <c r="AJ2" s="45"/>
-      <c r="AK2" s="45"/>
+      <c r="AI2" s="46"/>
+      <c r="AJ2" s="46"/>
+      <c r="AK2" s="46"/>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2267,23 +2267,23 @@
       <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="46"/>
-      <c r="M11" s="46"/>
-      <c r="N11" s="46"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
       <c r="O11" s="13"/>
       <c r="P11" s="13"/>
-      <c r="Q11" s="46"/>
-      <c r="R11" s="46"/>
+      <c r="Q11" s="47"/>
+      <c r="R11" s="47"/>
       <c r="S11" s="13"/>
       <c r="T11" s="13"/>
       <c r="U11" s="8"/>
@@ -2293,44 +2293,44 @@
       <c r="Z11" s="13"/>
       <c r="AA11" s="13"/>
       <c r="AB11" s="13"/>
-      <c r="AC11" s="46"/>
-      <c r="AD11" s="46"/>
+      <c r="AC11" s="47"/>
+      <c r="AD11" s="47"/>
       <c r="AE11" s="23"/>
       <c r="AF11" s="13"/>
       <c r="AG11" s="13"/>
       <c r="AH11" s="13"/>
-      <c r="AI11" s="46"/>
-      <c r="AJ11" s="46"/>
-      <c r="AK11" s="46"/>
+      <c r="AI11" s="47"/>
+      <c r="AJ11" s="47"/>
+      <c r="AK11" s="47"/>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
-      <c r="I12" s="45" t="s">
+      <c r="I12" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="J12" s="45"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="45"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="45"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="46"/>
+      <c r="M12" s="46"/>
+      <c r="N12" s="46"/>
+      <c r="O12" s="46"/>
       <c r="P12" s="13"/>
-      <c r="Q12" s="44" t="s">
+      <c r="Q12" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="R12" s="44"/>
-      <c r="S12" s="44"/>
+      <c r="R12" s="45"/>
+      <c r="S12" s="45"/>
       <c r="T12" s="13"/>
       <c r="U12" s="7" t="s">
         <v>65</v>
@@ -2347,21 +2347,21 @@
         <v>68</v>
       </c>
       <c r="AB12" s="13"/>
-      <c r="AC12" s="45" t="s">
+      <c r="AC12" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="AD12" s="45"/>
+      <c r="AD12" s="46"/>
       <c r="AE12" s="23"/>
       <c r="AF12" s="18" t="s">
         <v>70</v>
       </c>
       <c r="AG12" s="13"/>
-      <c r="AH12" s="45" t="s">
+      <c r="AH12" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="AI12" s="45"/>
-      <c r="AJ12" s="45"/>
-      <c r="AK12" s="45"/>
+      <c r="AI12" s="46"/>
+      <c r="AJ12" s="46"/>
+      <c r="AK12" s="46"/>
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -5475,40 +5475,40 @@
       <c r="A47" s="16"/>
       <c r="B47" s="13"/>
       <c r="C47" s="40"/>
-      <c r="D47" s="47" t="s">
+      <c r="D47" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="E47" s="47"/>
-      <c r="F47" s="47"/>
-      <c r="G47" s="47"/>
-      <c r="H47" s="47"/>
-      <c r="I47" s="47"/>
-      <c r="J47" s="47"/>
-      <c r="K47" s="47"/>
-      <c r="L47" s="47"/>
-      <c r="M47" s="47"/>
-      <c r="N47" s="47"/>
-      <c r="O47" s="47"/>
-      <c r="P47" s="47"/>
-      <c r="Q47" s="47"/>
-      <c r="R47" s="47"/>
-      <c r="S47" s="47"/>
-      <c r="T47" s="47"/>
-      <c r="U47" s="47"/>
-      <c r="V47" s="47"/>
-      <c r="W47" s="47"/>
-      <c r="X47" s="47"/>
-      <c r="Y47" s="47"/>
-      <c r="Z47" s="47"/>
-      <c r="AA47" s="47"/>
-      <c r="AB47" s="47"/>
-      <c r="AC47" s="47"/>
-      <c r="AD47" s="47"/>
-      <c r="AE47" s="47"/>
-      <c r="AF47" s="47"/>
-      <c r="AG47" s="47"/>
-      <c r="AH47" s="47"/>
-      <c r="AI47" s="47"/>
+      <c r="E47" s="48"/>
+      <c r="F47" s="48"/>
+      <c r="G47" s="48"/>
+      <c r="H47" s="48"/>
+      <c r="I47" s="48"/>
+      <c r="J47" s="48"/>
+      <c r="K47" s="48"/>
+      <c r="L47" s="48"/>
+      <c r="M47" s="48"/>
+      <c r="N47" s="48"/>
+      <c r="O47" s="48"/>
+      <c r="P47" s="48"/>
+      <c r="Q47" s="48"/>
+      <c r="R47" s="48"/>
+      <c r="S47" s="48"/>
+      <c r="T47" s="48"/>
+      <c r="U47" s="48"/>
+      <c r="V47" s="48"/>
+      <c r="W47" s="48"/>
+      <c r="X47" s="48"/>
+      <c r="Y47" s="48"/>
+      <c r="Z47" s="48"/>
+      <c r="AA47" s="48"/>
+      <c r="AB47" s="48"/>
+      <c r="AC47" s="48"/>
+      <c r="AD47" s="48"/>
+      <c r="AE47" s="48"/>
+      <c r="AF47" s="48"/>
+      <c r="AG47" s="48"/>
+      <c r="AH47" s="48"/>
+      <c r="AI47" s="48"/>
       <c r="AJ47" s="13"/>
       <c r="AK47" s="13"/>
       <c r="AL47"/>
@@ -5562,30 +5562,30 @@
       <c r="A49" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B49" s="44" t="s">
+      <c r="B49" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="C49" s="44"/>
-      <c r="D49" s="44"/>
-      <c r="E49" s="44"/>
+      <c r="C49" s="45"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="45"/>
       <c r="F49" s="20"/>
       <c r="G49" s="20"/>
       <c r="H49" s="20"/>
-      <c r="I49" s="45" t="s">
+      <c r="I49" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="J49" s="45"/>
-      <c r="K49" s="45"/>
-      <c r="L49" s="45"/>
-      <c r="M49" s="45"/>
-      <c r="N49" s="45"/>
-      <c r="O49" s="45"/>
+      <c r="J49" s="46"/>
+      <c r="K49" s="46"/>
+      <c r="L49" s="46"/>
+      <c r="M49" s="46"/>
+      <c r="N49" s="46"/>
+      <c r="O49" s="46"/>
       <c r="P49" s="13"/>
-      <c r="Q49" s="44" t="s">
+      <c r="Q49" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="R49" s="44"/>
-      <c r="S49" s="44"/>
+      <c r="R49" s="45"/>
+      <c r="S49" s="45"/>
       <c r="T49" s="13"/>
       <c r="U49" s="7" t="s">
         <v>65</v>
@@ -5602,21 +5602,21 @@
         <v>68</v>
       </c>
       <c r="AB49" s="13"/>
-      <c r="AC49" s="45" t="s">
+      <c r="AC49" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="AD49" s="45"/>
+      <c r="AD49" s="46"/>
       <c r="AE49" s="23"/>
       <c r="AF49" s="18" t="s">
         <v>70</v>
       </c>
       <c r="AG49" s="13"/>
-      <c r="AH49" s="45" t="s">
+      <c r="AH49" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="AI49" s="45"/>
-      <c r="AJ49" s="45"/>
-      <c r="AK49" s="45"/>
+      <c r="AI49" s="46"/>
+      <c r="AJ49" s="46"/>
+      <c r="AK49" s="46"/>
     </row>
     <row r="50" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
@@ -8139,30 +8139,30 @@
       <c r="A81" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B81" s="44" t="s">
+      <c r="B81" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="C81" s="44"/>
-      <c r="D81" s="44"/>
-      <c r="E81" s="44"/>
+      <c r="C81" s="45"/>
+      <c r="D81" s="45"/>
+      <c r="E81" s="45"/>
       <c r="F81" s="20"/>
       <c r="G81" s="20"/>
       <c r="H81" s="20"/>
-      <c r="I81" s="45" t="s">
+      <c r="I81" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="J81" s="45"/>
-      <c r="K81" s="45"/>
-      <c r="L81" s="45"/>
-      <c r="M81" s="45"/>
-      <c r="N81" s="45"/>
-      <c r="O81" s="45"/>
+      <c r="J81" s="46"/>
+      <c r="K81" s="46"/>
+      <c r="L81" s="46"/>
+      <c r="M81" s="46"/>
+      <c r="N81" s="46"/>
+      <c r="O81" s="46"/>
       <c r="P81" s="13"/>
-      <c r="Q81" s="44" t="s">
+      <c r="Q81" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="R81" s="44"/>
-      <c r="S81" s="44"/>
+      <c r="R81" s="45"/>
+      <c r="S81" s="45"/>
       <c r="T81" s="13"/>
       <c r="U81" s="7" t="s">
         <v>65</v>
@@ -8179,21 +8179,21 @@
         <v>68</v>
       </c>
       <c r="AB81" s="13"/>
-      <c r="AC81" s="45" t="s">
+      <c r="AC81" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="AD81" s="45"/>
+      <c r="AD81" s="46"/>
       <c r="AE81" s="23"/>
       <c r="AF81" s="18" t="s">
         <v>70</v>
       </c>
       <c r="AG81" s="13"/>
-      <c r="AH81" s="45" t="s">
+      <c r="AH81" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="AI81" s="45"/>
-      <c r="AJ81" s="45"/>
-      <c r="AK81" s="45"/>
+      <c r="AI81" s="46"/>
+      <c r="AJ81" s="46"/>
+      <c r="AK81" s="46"/>
     </row>
     <row r="82" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
@@ -10633,7 +10633,7 @@
       </c>
     </row>
     <row r="111" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A111" s="48" t="s">
+      <c r="A111" s="44" t="s">
         <v>187</v>
       </c>
       <c r="B111" s="35" t="s">
@@ -10768,30 +10768,30 @@
       <c r="A113" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B113" s="44" t="s">
+      <c r="B113" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="C113" s="44"/>
-      <c r="D113" s="44"/>
-      <c r="E113" s="44"/>
+      <c r="C113" s="45"/>
+      <c r="D113" s="45"/>
+      <c r="E113" s="45"/>
       <c r="F113" s="20"/>
       <c r="G113" s="20"/>
       <c r="H113" s="20"/>
-      <c r="I113" s="45" t="s">
+      <c r="I113" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="J113" s="45"/>
-      <c r="K113" s="45"/>
-      <c r="L113" s="45"/>
-      <c r="M113" s="45"/>
-      <c r="N113" s="45"/>
-      <c r="O113" s="45"/>
+      <c r="J113" s="46"/>
+      <c r="K113" s="46"/>
+      <c r="L113" s="46"/>
+      <c r="M113" s="46"/>
+      <c r="N113" s="46"/>
+      <c r="O113" s="46"/>
       <c r="P113" s="13"/>
-      <c r="Q113" s="44" t="s">
+      <c r="Q113" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="R113" s="44"/>
-      <c r="S113" s="44"/>
+      <c r="R113" s="45"/>
+      <c r="S113" s="45"/>
       <c r="T113" s="13"/>
       <c r="U113" s="7" t="s">
         <v>65</v>
@@ -10808,21 +10808,21 @@
         <v>68</v>
       </c>
       <c r="AB113" s="13"/>
-      <c r="AC113" s="45" t="s">
+      <c r="AC113" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="AD113" s="45"/>
+      <c r="AD113" s="46"/>
       <c r="AE113" s="23"/>
       <c r="AF113" s="18" t="s">
         <v>70</v>
       </c>
       <c r="AG113" s="13"/>
-      <c r="AH113" s="45" t="s">
+      <c r="AH113" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="AI113" s="45"/>
-      <c r="AJ113" s="45"/>
-      <c r="AK113" s="45"/>
+      <c r="AI113" s="46"/>
+      <c r="AJ113" s="46"/>
+      <c r="AK113" s="46"/>
     </row>
     <row r="114" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
@@ -12199,30 +12199,30 @@
       <c r="A131" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B131" s="44" t="s">
+      <c r="B131" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="C131" s="44"/>
-      <c r="D131" s="44"/>
-      <c r="E131" s="44"/>
+      <c r="C131" s="45"/>
+      <c r="D131" s="45"/>
+      <c r="E131" s="45"/>
       <c r="F131" s="20"/>
       <c r="G131" s="20"/>
       <c r="H131" s="20"/>
-      <c r="I131" s="45" t="s">
+      <c r="I131" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="J131" s="45"/>
-      <c r="K131" s="45"/>
-      <c r="L131" s="45"/>
-      <c r="M131" s="45"/>
-      <c r="N131" s="45"/>
-      <c r="O131" s="45"/>
+      <c r="J131" s="46"/>
+      <c r="K131" s="46"/>
+      <c r="L131" s="46"/>
+      <c r="M131" s="46"/>
+      <c r="N131" s="46"/>
+      <c r="O131" s="46"/>
       <c r="P131" s="13"/>
-      <c r="Q131" s="44" t="s">
+      <c r="Q131" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="R131" s="44"/>
-      <c r="S131" s="44"/>
+      <c r="R131" s="45"/>
+      <c r="S131" s="45"/>
       <c r="T131" s="13"/>
       <c r="U131" s="7" t="s">
         <v>65</v>
@@ -12239,21 +12239,21 @@
         <v>68</v>
       </c>
       <c r="AB131" s="13"/>
-      <c r="AC131" s="45" t="s">
+      <c r="AC131" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="AD131" s="45"/>
+      <c r="AD131" s="46"/>
       <c r="AE131" s="23"/>
       <c r="AF131" s="18" t="s">
         <v>70</v>
       </c>
       <c r="AG131" s="13"/>
-      <c r="AH131" s="45" t="s">
+      <c r="AH131" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="AI131" s="45"/>
-      <c r="AJ131" s="45"/>
-      <c r="AK131" s="45"/>
+      <c r="AI131" s="46"/>
+      <c r="AJ131" s="46"/>
+      <c r="AK131" s="46"/>
     </row>
     <row r="132" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
@@ -13547,7 +13547,7 @@
       </c>
     </row>
     <row r="147" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A147" s="48" t="s">
+      <c r="A147" s="44" t="s">
         <v>188</v>
       </c>
       <c r="B147" s="35" t="s">
@@ -13643,30 +13643,30 @@
       <c r="A148" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B148" s="44" t="s">
+      <c r="B148" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="C148" s="44"/>
-      <c r="D148" s="44"/>
-      <c r="E148" s="44"/>
+      <c r="C148" s="45"/>
+      <c r="D148" s="45"/>
+      <c r="E148" s="45"/>
       <c r="F148" s="20"/>
       <c r="G148" s="20"/>
       <c r="H148" s="20"/>
-      <c r="I148" s="45" t="s">
+      <c r="I148" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="J148" s="45"/>
-      <c r="K148" s="45"/>
-      <c r="L148" s="45"/>
-      <c r="M148" s="45"/>
-      <c r="N148" s="45"/>
-      <c r="O148" s="45"/>
+      <c r="J148" s="46"/>
+      <c r="K148" s="46"/>
+      <c r="L148" s="46"/>
+      <c r="M148" s="46"/>
+      <c r="N148" s="46"/>
+      <c r="O148" s="46"/>
       <c r="P148" s="13"/>
-      <c r="Q148" s="44" t="s">
+      <c r="Q148" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="R148" s="44"/>
-      <c r="S148" s="44"/>
+      <c r="R148" s="45"/>
+      <c r="S148" s="45"/>
       <c r="T148" s="13"/>
       <c r="U148" s="7" t="s">
         <v>65</v>
@@ -13683,21 +13683,21 @@
         <v>68</v>
       </c>
       <c r="AB148" s="13"/>
-      <c r="AC148" s="45" t="s">
+      <c r="AC148" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="AD148" s="45"/>
+      <c r="AD148" s="46"/>
       <c r="AE148" s="23"/>
       <c r="AF148" s="18" t="s">
         <v>70</v>
       </c>
       <c r="AG148" s="13"/>
-      <c r="AH148" s="45" t="s">
+      <c r="AH148" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="AI148" s="45"/>
-      <c r="AJ148" s="45"/>
-      <c r="AK148" s="45"/>
+      <c r="AI148" s="46"/>
+      <c r="AJ148" s="46"/>
+      <c r="AK148" s="46"/>
     </row>
     <row r="149" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
@@ -13928,30 +13928,30 @@
       <c r="A152" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B152" s="44" t="s">
+      <c r="B152" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="C152" s="44"/>
-      <c r="D152" s="44"/>
-      <c r="E152" s="44"/>
+      <c r="C152" s="45"/>
+      <c r="D152" s="45"/>
+      <c r="E152" s="45"/>
       <c r="F152" s="20"/>
       <c r="G152" s="20"/>
       <c r="H152" s="20"/>
-      <c r="I152" s="45" t="s">
+      <c r="I152" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="J152" s="45"/>
-      <c r="K152" s="45"/>
-      <c r="L152" s="45"/>
-      <c r="M152" s="45"/>
-      <c r="N152" s="45"/>
-      <c r="O152" s="45"/>
+      <c r="J152" s="46"/>
+      <c r="K152" s="46"/>
+      <c r="L152" s="46"/>
+      <c r="M152" s="46"/>
+      <c r="N152" s="46"/>
+      <c r="O152" s="46"/>
       <c r="P152" s="13"/>
-      <c r="Q152" s="44" t="s">
+      <c r="Q152" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="R152" s="44"/>
-      <c r="S152" s="44"/>
+      <c r="R152" s="45"/>
+      <c r="S152" s="45"/>
       <c r="T152" s="13"/>
       <c r="U152" s="7" t="s">
         <v>65</v>
@@ -13968,21 +13968,21 @@
         <v>68</v>
       </c>
       <c r="AB152" s="13"/>
-      <c r="AC152" s="45" t="s">
+      <c r="AC152" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="AD152" s="45"/>
+      <c r="AD152" s="46"/>
       <c r="AE152" s="23"/>
       <c r="AF152" s="18" t="s">
         <v>70</v>
       </c>
       <c r="AG152" s="13"/>
-      <c r="AH152" s="45" t="s">
+      <c r="AH152" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="AI152" s="45"/>
-      <c r="AJ152" s="45"/>
-      <c r="AK152" s="45"/>
+      <c r="AI152" s="46"/>
+      <c r="AJ152" s="46"/>
+      <c r="AK152" s="46"/>
     </row>
     <row r="153" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
@@ -14212,30 +14212,30 @@
       <c r="A156" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B156" s="44" t="s">
+      <c r="B156" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="C156" s="44"/>
-      <c r="D156" s="44"/>
-      <c r="E156" s="44"/>
+      <c r="C156" s="45"/>
+      <c r="D156" s="45"/>
+      <c r="E156" s="45"/>
       <c r="F156" s="20"/>
       <c r="G156" s="20"/>
       <c r="H156" s="20"/>
-      <c r="I156" s="45" t="s">
+      <c r="I156" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="J156" s="45"/>
-      <c r="K156" s="45"/>
-      <c r="L156" s="45"/>
-      <c r="M156" s="45"/>
-      <c r="N156" s="45"/>
-      <c r="O156" s="45"/>
+      <c r="J156" s="46"/>
+      <c r="K156" s="46"/>
+      <c r="L156" s="46"/>
+      <c r="M156" s="46"/>
+      <c r="N156" s="46"/>
+      <c r="O156" s="46"/>
       <c r="P156" s="13"/>
-      <c r="Q156" s="44" t="s">
+      <c r="Q156" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="R156" s="44"/>
-      <c r="S156" s="44"/>
+      <c r="R156" s="45"/>
+      <c r="S156" s="45"/>
       <c r="T156" s="13"/>
       <c r="U156" s="7" t="s">
         <v>65</v>
@@ -14252,21 +14252,21 @@
         <v>68</v>
       </c>
       <c r="AB156" s="13"/>
-      <c r="AC156" s="45" t="s">
+      <c r="AC156" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="AD156" s="45"/>
+      <c r="AD156" s="46"/>
       <c r="AE156" s="23"/>
       <c r="AF156" s="18" t="s">
         <v>70</v>
       </c>
       <c r="AG156" s="13"/>
-      <c r="AH156" s="45" t="s">
+      <c r="AH156" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="AI156" s="45"/>
-      <c r="AJ156" s="45"/>
-      <c r="AK156" s="45"/>
+      <c r="AI156" s="46"/>
+      <c r="AJ156" s="46"/>
+      <c r="AK156" s="46"/>
     </row>
     <row r="157" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
@@ -14449,30 +14449,30 @@
       <c r="A160" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B160" s="44" t="s">
+      <c r="B160" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="C160" s="44"/>
-      <c r="D160" s="44"/>
-      <c r="E160" s="44"/>
+      <c r="C160" s="45"/>
+      <c r="D160" s="45"/>
+      <c r="E160" s="45"/>
       <c r="F160" s="20"/>
       <c r="G160" s="20"/>
       <c r="H160" s="20"/>
-      <c r="I160" s="45" t="s">
+      <c r="I160" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="J160" s="45"/>
-      <c r="K160" s="45"/>
-      <c r="L160" s="45"/>
-      <c r="M160" s="45"/>
-      <c r="N160" s="45"/>
-      <c r="O160" s="45"/>
+      <c r="J160" s="46"/>
+      <c r="K160" s="46"/>
+      <c r="L160" s="46"/>
+      <c r="M160" s="46"/>
+      <c r="N160" s="46"/>
+      <c r="O160" s="46"/>
       <c r="P160" s="13"/>
-      <c r="Q160" s="44" t="s">
+      <c r="Q160" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="R160" s="44"/>
-      <c r="S160" s="44"/>
+      <c r="R160" s="45"/>
+      <c r="S160" s="45"/>
       <c r="T160" s="13"/>
       <c r="U160" s="7" t="s">
         <v>65</v>
@@ -14489,21 +14489,21 @@
         <v>68</v>
       </c>
       <c r="AB160" s="13"/>
-      <c r="AC160" s="45" t="s">
+      <c r="AC160" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="AD160" s="45"/>
+      <c r="AD160" s="46"/>
       <c r="AE160" s="23"/>
       <c r="AF160" s="18" t="s">
         <v>70</v>
       </c>
       <c r="AG160" s="13"/>
-      <c r="AH160" s="45" t="s">
+      <c r="AH160" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="AI160" s="45"/>
-      <c r="AJ160" s="45"/>
-      <c r="AK160" s="45"/>
+      <c r="AI160" s="46"/>
+      <c r="AJ160" s="46"/>
+      <c r="AK160" s="46"/>
     </row>
     <row r="161" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
@@ -14830,17 +14830,35 @@
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="B148:E148"/>
-    <mergeCell ref="B152:E152"/>
-    <mergeCell ref="I81:O81"/>
-    <mergeCell ref="I113:O113"/>
-    <mergeCell ref="I131:O131"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="I11:N11"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="I12:O12"/>
+    <mergeCell ref="B160:E160"/>
+    <mergeCell ref="AC160:AD160"/>
+    <mergeCell ref="AH160:AK160"/>
+    <mergeCell ref="I160:O160"/>
+    <mergeCell ref="Q160:S160"/>
+    <mergeCell ref="B156:E156"/>
+    <mergeCell ref="AC156:AD156"/>
+    <mergeCell ref="AH156:AK156"/>
+    <mergeCell ref="I156:O156"/>
+    <mergeCell ref="Q156:S156"/>
+    <mergeCell ref="AH12:AK12"/>
+    <mergeCell ref="AH49:AK49"/>
+    <mergeCell ref="AI11:AK11"/>
+    <mergeCell ref="AC113:AD113"/>
+    <mergeCell ref="Q148:S148"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="Q49:S49"/>
+    <mergeCell ref="AC12:AD12"/>
+    <mergeCell ref="AH131:AK131"/>
+    <mergeCell ref="AC131:AD131"/>
+    <mergeCell ref="AC81:AD81"/>
+    <mergeCell ref="Q81:S81"/>
+    <mergeCell ref="Q113:S113"/>
+    <mergeCell ref="Q131:S131"/>
+    <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="AC11:AD11"/>
     <mergeCell ref="AC152:AD152"/>
     <mergeCell ref="D47:AI47"/>
     <mergeCell ref="AC49:AD49"/>
@@ -14857,35 +14875,17 @@
     <mergeCell ref="AH81:AK81"/>
     <mergeCell ref="B113:E113"/>
     <mergeCell ref="AH113:AK113"/>
-    <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="AC11:AD11"/>
-    <mergeCell ref="AH12:AK12"/>
-    <mergeCell ref="AH49:AK49"/>
-    <mergeCell ref="AI11:AK11"/>
-    <mergeCell ref="AC113:AD113"/>
-    <mergeCell ref="Q148:S148"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="Q49:S49"/>
-    <mergeCell ref="AC12:AD12"/>
-    <mergeCell ref="AH131:AK131"/>
-    <mergeCell ref="AC131:AD131"/>
-    <mergeCell ref="AC81:AD81"/>
-    <mergeCell ref="Q81:S81"/>
-    <mergeCell ref="Q113:S113"/>
-    <mergeCell ref="Q131:S131"/>
-    <mergeCell ref="B156:E156"/>
-    <mergeCell ref="AC156:AD156"/>
-    <mergeCell ref="AH156:AK156"/>
-    <mergeCell ref="I156:O156"/>
-    <mergeCell ref="Q156:S156"/>
-    <mergeCell ref="B160:E160"/>
-    <mergeCell ref="AC160:AD160"/>
-    <mergeCell ref="AH160:AK160"/>
-    <mergeCell ref="I160:O160"/>
-    <mergeCell ref="Q160:S160"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="I11:N11"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="I12:O12"/>
+    <mergeCell ref="B148:E148"/>
+    <mergeCell ref="B152:E152"/>
+    <mergeCell ref="I81:O81"/>
+    <mergeCell ref="I113:O113"/>
+    <mergeCell ref="I131:O131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="44" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>